<commit_message>
Fix Drivers+Proactiva in paralell, fix stage 3 of workflow
</commit_message>
<xml_diff>
--- a/devops-powershell/reportes/templete/Checklist Proactiva Actualizada - Cliente - Mes.xlsx
+++ b/devops-powershell/reportes/templete/Checklist Proactiva Actualizada - Cliente - Mes.xlsx
@@ -5,7 +5,7 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\SALV\Desktop\trabajo\Pruebas Scripts\proactivas\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\SALV\Desktop\PROACTIVAS\PROACTIVAS\wpc-proactivas-portable v2.0.1ovw\devops-powershell\reportes\templete\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -776,12 +776,6 @@
       <name val="Calibri"/>
     </font>
     <font>
-      <u/>
-      <sz val="11"/>
-      <color theme="10"/>
-      <name val="Calibri"/>
-    </font>
-    <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
       <name val="Arial"/>
@@ -795,6 +789,12 @@
       <sz val="10"/>
       <color rgb="FF000000"/>
       <name val="Roboto"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="6">
@@ -1001,8 +1001,7 @@
     <xf numFmtId="0" fontId="2" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="5" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1029,7 +1028,7 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -1037,7 +1036,7 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -1047,7 +1046,7 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -1078,9 +1077,10 @@
     <xf numFmtId="0" fontId="2" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyProtection="1"/>
+    <xf numFmtId="0" fontId="8" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1298,8 +1298,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Z987"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E1" workbookViewId="0">
-      <selection activeCell="H9" sqref="H9"/>
+    <sheetView tabSelected="1" topLeftCell="C3" workbookViewId="0">
+      <selection activeCell="G15" sqref="G15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
@@ -1364,7 +1364,7 @@
         <v>14</v>
       </c>
       <c r="G2" s="5"/>
-      <c r="H2" s="55"/>
+      <c r="H2" s="54"/>
       <c r="I2" s="4"/>
       <c r="J2" s="6"/>
       <c r="K2" s="6"/>
@@ -1844,8 +1844,8 @@
         <v>36</v>
       </c>
       <c r="G14" s="19"/>
-      <c r="H14" s="22"/>
-      <c r="I14" s="23"/>
+      <c r="H14" s="55"/>
+      <c r="I14" s="22"/>
       <c r="J14" s="20"/>
       <c r="K14" s="20"/>
       <c r="L14" s="20"/>
@@ -2025,27 +2025,27 @@
       <c r="Z18" s="20"/>
     </row>
     <row r="19" spans="1:26">
-      <c r="A19" s="24" t="s">
+      <c r="A19" s="23" t="s">
         <v>52</v>
       </c>
-      <c r="B19" s="25" t="s">
+      <c r="B19" s="24" t="s">
         <v>10</v>
       </c>
-      <c r="C19" s="26" t="s">
+      <c r="C19" s="25" t="s">
         <v>11</v>
       </c>
-      <c r="D19" s="26" t="s">
+      <c r="D19" s="25" t="s">
         <v>12</v>
       </c>
-      <c r="E19" s="25" t="s">
+      <c r="E19" s="24" t="s">
         <v>53</v>
       </c>
-      <c r="F19" s="27" t="s">
+      <c r="F19" s="26" t="s">
         <v>36</v>
       </c>
-      <c r="G19" s="26"/>
-      <c r="H19" s="26"/>
-      <c r="I19" s="25"/>
+      <c r="G19" s="25"/>
+      <c r="H19" s="25"/>
+      <c r="I19" s="24"/>
       <c r="J19" s="20"/>
       <c r="K19" s="20"/>
       <c r="L19" s="20"/>
@@ -2065,27 +2065,27 @@
       <c r="Z19" s="20"/>
     </row>
     <row r="20" spans="1:26" ht="15" customHeight="1">
-      <c r="A20" s="28" t="s">
+      <c r="A20" s="27" t="s">
         <v>54</v>
       </c>
-      <c r="B20" s="29" t="s">
+      <c r="B20" s="28" t="s">
         <v>10</v>
       </c>
-      <c r="C20" s="30" t="s">
+      <c r="C20" s="29" t="s">
         <v>55</v>
       </c>
-      <c r="D20" s="30" t="s">
+      <c r="D20" s="29" t="s">
         <v>12</v>
       </c>
-      <c r="E20" s="29" t="s">
+      <c r="E20" s="28" t="s">
         <v>56</v>
       </c>
-      <c r="F20" s="29" t="s">
+      <c r="F20" s="28" t="s">
         <v>14</v>
       </c>
-      <c r="G20" s="30"/>
-      <c r="H20" s="30"/>
-      <c r="I20" s="29"/>
+      <c r="G20" s="29"/>
+      <c r="H20" s="29"/>
+      <c r="I20" s="28"/>
       <c r="J20" s="20"/>
       <c r="K20" s="20"/>
       <c r="L20" s="20"/>
@@ -2505,27 +2505,27 @@
       <c r="Z30" s="20"/>
     </row>
     <row r="31" spans="1:26" ht="15.75" customHeight="1">
-      <c r="A31" s="24" t="s">
+      <c r="A31" s="23" t="s">
         <v>77</v>
       </c>
-      <c r="B31" s="25" t="s">
+      <c r="B31" s="24" t="s">
         <v>10</v>
       </c>
-      <c r="C31" s="26" t="s">
+      <c r="C31" s="25" t="s">
         <v>55</v>
       </c>
-      <c r="D31" s="26" t="s">
+      <c r="D31" s="25" t="s">
         <v>12</v>
       </c>
-      <c r="E31" s="25" t="s">
+      <c r="E31" s="24" t="s">
         <v>78</v>
       </c>
-      <c r="F31" s="25" t="s">
+      <c r="F31" s="24" t="s">
         <v>36</v>
       </c>
-      <c r="G31" s="26"/>
-      <c r="H31" s="26"/>
-      <c r="I31" s="25"/>
+      <c r="G31" s="25"/>
+      <c r="H31" s="25"/>
+      <c r="I31" s="24"/>
       <c r="J31" s="20"/>
       <c r="K31" s="20"/>
       <c r="L31" s="20"/>
@@ -2545,27 +2545,27 @@
       <c r="Z31" s="20"/>
     </row>
     <row r="32" spans="1:26" ht="15.75" customHeight="1">
-      <c r="A32" s="28" t="s">
+      <c r="A32" s="27" t="s">
         <v>79</v>
       </c>
-      <c r="B32" s="29" t="s">
+      <c r="B32" s="28" t="s">
         <v>10</v>
       </c>
-      <c r="C32" s="30" t="s">
+      <c r="C32" s="29" t="s">
         <v>80</v>
       </c>
-      <c r="D32" s="30" t="s">
+      <c r="D32" s="29" t="s">
         <v>12</v>
       </c>
-      <c r="E32" s="29" t="s">
+      <c r="E32" s="28" t="s">
         <v>81</v>
       </c>
-      <c r="F32" s="29" t="s">
+      <c r="F32" s="28" t="s">
         <v>36</v>
       </c>
-      <c r="G32" s="30"/>
-      <c r="H32" s="30"/>
-      <c r="I32" s="29"/>
+      <c r="G32" s="29"/>
+      <c r="H32" s="29"/>
+      <c r="I32" s="28"/>
       <c r="J32" s="20"/>
       <c r="K32" s="20"/>
       <c r="L32" s="20"/>
@@ -2625,764 +2625,764 @@
       <c r="Z33" s="20"/>
     </row>
     <row r="34" spans="1:26" ht="15.75" customHeight="1">
-      <c r="A34" s="31" t="s">
+      <c r="A34" s="30" t="s">
         <v>84</v>
       </c>
-      <c r="B34" s="32" t="s">
+      <c r="B34" s="31" t="s">
         <v>85</v>
       </c>
-      <c r="C34" s="33" t="s">
+      <c r="C34" s="32" t="s">
         <v>11</v>
       </c>
-      <c r="D34" s="33" t="s">
+      <c r="D34" s="32" t="s">
         <v>34</v>
       </c>
-      <c r="E34" s="34" t="s">
+      <c r="E34" s="33" t="s">
         <v>86</v>
       </c>
-      <c r="F34" s="35" t="s">
+      <c r="F34" s="34" t="s">
         <v>14</v>
       </c>
-      <c r="G34" s="33"/>
-      <c r="H34" s="33"/>
-      <c r="I34" s="32"/>
-      <c r="J34" s="36"/>
-      <c r="K34" s="36"/>
-      <c r="L34" s="36"/>
-      <c r="M34" s="36"/>
-      <c r="N34" s="36"/>
-      <c r="O34" s="36"/>
-      <c r="P34" s="36"/>
-      <c r="Q34" s="36"/>
-      <c r="R34" s="36"/>
-      <c r="S34" s="36"/>
-      <c r="T34" s="36"/>
-      <c r="U34" s="36"/>
-      <c r="V34" s="36"/>
-      <c r="W34" s="36"/>
-      <c r="X34" s="36"/>
-      <c r="Y34" s="36"/>
-      <c r="Z34" s="36"/>
+      <c r="G34" s="32"/>
+      <c r="H34" s="32"/>
+      <c r="I34" s="31"/>
+      <c r="J34" s="35"/>
+      <c r="K34" s="35"/>
+      <c r="L34" s="35"/>
+      <c r="M34" s="35"/>
+      <c r="N34" s="35"/>
+      <c r="O34" s="35"/>
+      <c r="P34" s="35"/>
+      <c r="Q34" s="35"/>
+      <c r="R34" s="35"/>
+      <c r="S34" s="35"/>
+      <c r="T34" s="35"/>
+      <c r="U34" s="35"/>
+      <c r="V34" s="35"/>
+      <c r="W34" s="35"/>
+      <c r="X34" s="35"/>
+      <c r="Y34" s="35"/>
+      <c r="Z34" s="35"/>
     </row>
     <row r="35" spans="1:26" ht="15.75" customHeight="1">
-      <c r="A35" s="31" t="s">
+      <c r="A35" s="30" t="s">
         <v>87</v>
       </c>
-      <c r="B35" s="32" t="s">
+      <c r="B35" s="31" t="s">
         <v>85</v>
       </c>
-      <c r="C35" s="33" t="s">
+      <c r="C35" s="32" t="s">
         <v>11</v>
       </c>
-      <c r="D35" s="33" t="s">
+      <c r="D35" s="32" t="s">
         <v>34</v>
       </c>
-      <c r="E35" s="34" t="s">
+      <c r="E35" s="33" t="s">
         <v>88</v>
       </c>
-      <c r="F35" s="35" t="s">
+      <c r="F35" s="34" t="s">
         <v>21</v>
       </c>
-      <c r="G35" s="33"/>
-      <c r="H35" s="33"/>
-      <c r="I35" s="32"/>
-      <c r="J35" s="36"/>
-      <c r="K35" s="36"/>
-      <c r="L35" s="36"/>
-      <c r="M35" s="36"/>
-      <c r="N35" s="36"/>
-      <c r="O35" s="36"/>
-      <c r="P35" s="36"/>
-      <c r="Q35" s="36"/>
-      <c r="R35" s="36"/>
-      <c r="S35" s="36"/>
-      <c r="T35" s="36"/>
-      <c r="U35" s="36"/>
-      <c r="V35" s="36"/>
-      <c r="W35" s="36"/>
-      <c r="X35" s="36"/>
-      <c r="Y35" s="36"/>
-      <c r="Z35" s="36"/>
+      <c r="G35" s="32"/>
+      <c r="H35" s="32"/>
+      <c r="I35" s="31"/>
+      <c r="J35" s="35"/>
+      <c r="K35" s="35"/>
+      <c r="L35" s="35"/>
+      <c r="M35" s="35"/>
+      <c r="N35" s="35"/>
+      <c r="O35" s="35"/>
+      <c r="P35" s="35"/>
+      <c r="Q35" s="35"/>
+      <c r="R35" s="35"/>
+      <c r="S35" s="35"/>
+      <c r="T35" s="35"/>
+      <c r="U35" s="35"/>
+      <c r="V35" s="35"/>
+      <c r="W35" s="35"/>
+      <c r="X35" s="35"/>
+      <c r="Y35" s="35"/>
+      <c r="Z35" s="35"/>
     </row>
     <row r="36" spans="1:26" ht="15.75" customHeight="1">
-      <c r="A36" s="31" t="s">
+      <c r="A36" s="30" t="s">
         <v>89</v>
       </c>
-      <c r="B36" s="32" t="s">
+      <c r="B36" s="31" t="s">
         <v>85</v>
       </c>
-      <c r="C36" s="33" t="s">
+      <c r="C36" s="32" t="s">
         <v>11</v>
       </c>
-      <c r="D36" s="33" t="s">
+      <c r="D36" s="32" t="s">
         <v>34</v>
       </c>
-      <c r="E36" s="34" t="s">
+      <c r="E36" s="33" t="s">
         <v>90</v>
       </c>
-      <c r="F36" s="35" t="s">
+      <c r="F36" s="34" t="s">
         <v>36</v>
       </c>
-      <c r="G36" s="33"/>
-      <c r="H36" s="33"/>
-      <c r="I36" s="32"/>
-      <c r="J36" s="36"/>
-      <c r="K36" s="36"/>
-      <c r="L36" s="36"/>
-      <c r="M36" s="36"/>
-      <c r="N36" s="36"/>
-      <c r="O36" s="36"/>
-      <c r="P36" s="36"/>
-      <c r="Q36" s="36"/>
-      <c r="R36" s="36"/>
-      <c r="S36" s="36"/>
-      <c r="T36" s="36"/>
-      <c r="U36" s="36"/>
-      <c r="V36" s="36"/>
-      <c r="W36" s="36"/>
-      <c r="X36" s="36"/>
-      <c r="Y36" s="36"/>
-      <c r="Z36" s="36"/>
+      <c r="G36" s="32"/>
+      <c r="H36" s="32"/>
+      <c r="I36" s="31"/>
+      <c r="J36" s="35"/>
+      <c r="K36" s="35"/>
+      <c r="L36" s="35"/>
+      <c r="M36" s="35"/>
+      <c r="N36" s="35"/>
+      <c r="O36" s="35"/>
+      <c r="P36" s="35"/>
+      <c r="Q36" s="35"/>
+      <c r="R36" s="35"/>
+      <c r="S36" s="35"/>
+      <c r="T36" s="35"/>
+      <c r="U36" s="35"/>
+      <c r="V36" s="35"/>
+      <c r="W36" s="35"/>
+      <c r="X36" s="35"/>
+      <c r="Y36" s="35"/>
+      <c r="Z36" s="35"/>
     </row>
     <row r="37" spans="1:26" ht="15.75" customHeight="1">
-      <c r="A37" s="31" t="s">
+      <c r="A37" s="30" t="s">
         <v>91</v>
       </c>
-      <c r="B37" s="32" t="s">
+      <c r="B37" s="31" t="s">
         <v>85</v>
       </c>
-      <c r="C37" s="33" t="s">
+      <c r="C37" s="32" t="s">
         <v>11</v>
       </c>
-      <c r="D37" s="33" t="s">
+      <c r="D37" s="32" t="s">
         <v>34</v>
       </c>
-      <c r="E37" s="34" t="s">
+      <c r="E37" s="33" t="s">
         <v>92</v>
       </c>
-      <c r="F37" s="35" t="s">
+      <c r="F37" s="34" t="s">
         <v>36</v>
       </c>
-      <c r="G37" s="33"/>
-      <c r="H37" s="33"/>
-      <c r="I37" s="32"/>
-      <c r="J37" s="36"/>
-      <c r="K37" s="36"/>
-      <c r="L37" s="36"/>
-      <c r="M37" s="36"/>
-      <c r="N37" s="36"/>
-      <c r="O37" s="36"/>
-      <c r="P37" s="36"/>
-      <c r="Q37" s="36"/>
-      <c r="R37" s="36"/>
-      <c r="S37" s="36"/>
-      <c r="T37" s="36"/>
-      <c r="U37" s="36"/>
-      <c r="V37" s="36"/>
-      <c r="W37" s="36"/>
-      <c r="X37" s="36"/>
-      <c r="Y37" s="36"/>
-      <c r="Z37" s="36"/>
+      <c r="G37" s="32"/>
+      <c r="H37" s="32"/>
+      <c r="I37" s="31"/>
+      <c r="J37" s="35"/>
+      <c r="K37" s="35"/>
+      <c r="L37" s="35"/>
+      <c r="M37" s="35"/>
+      <c r="N37" s="35"/>
+      <c r="O37" s="35"/>
+      <c r="P37" s="35"/>
+      <c r="Q37" s="35"/>
+      <c r="R37" s="35"/>
+      <c r="S37" s="35"/>
+      <c r="T37" s="35"/>
+      <c r="U37" s="35"/>
+      <c r="V37" s="35"/>
+      <c r="W37" s="35"/>
+      <c r="X37" s="35"/>
+      <c r="Y37" s="35"/>
+      <c r="Z37" s="35"/>
     </row>
     <row r="38" spans="1:26" ht="15.75" customHeight="1">
-      <c r="A38" s="31" t="s">
+      <c r="A38" s="30" t="s">
         <v>93</v>
       </c>
-      <c r="B38" s="32" t="s">
+      <c r="B38" s="31" t="s">
         <v>85</v>
       </c>
-      <c r="C38" s="33" t="s">
+      <c r="C38" s="32" t="s">
         <v>11</v>
       </c>
-      <c r="D38" s="33" t="s">
+      <c r="D38" s="32" t="s">
         <v>34</v>
       </c>
-      <c r="E38" s="34" t="s">
+      <c r="E38" s="33" t="s">
         <v>94</v>
       </c>
-      <c r="F38" s="35" t="s">
+      <c r="F38" s="34" t="s">
         <v>36</v>
       </c>
-      <c r="G38" s="33"/>
-      <c r="H38" s="33"/>
-      <c r="I38" s="32"/>
-      <c r="J38" s="36"/>
-      <c r="K38" s="36"/>
-      <c r="L38" s="36"/>
-      <c r="M38" s="36"/>
-      <c r="N38" s="36"/>
-      <c r="O38" s="36"/>
-      <c r="P38" s="36"/>
-      <c r="Q38" s="36"/>
-      <c r="R38" s="36"/>
-      <c r="S38" s="36"/>
-      <c r="T38" s="36"/>
-      <c r="U38" s="36"/>
-      <c r="V38" s="36"/>
-      <c r="W38" s="36"/>
-      <c r="X38" s="36"/>
-      <c r="Y38" s="36"/>
-      <c r="Z38" s="36"/>
+      <c r="G38" s="32"/>
+      <c r="H38" s="32"/>
+      <c r="I38" s="31"/>
+      <c r="J38" s="35"/>
+      <c r="K38" s="35"/>
+      <c r="L38" s="35"/>
+      <c r="M38" s="35"/>
+      <c r="N38" s="35"/>
+      <c r="O38" s="35"/>
+      <c r="P38" s="35"/>
+      <c r="Q38" s="35"/>
+      <c r="R38" s="35"/>
+      <c r="S38" s="35"/>
+      <c r="T38" s="35"/>
+      <c r="U38" s="35"/>
+      <c r="V38" s="35"/>
+      <c r="W38" s="35"/>
+      <c r="X38" s="35"/>
+      <c r="Y38" s="35"/>
+      <c r="Z38" s="35"/>
     </row>
     <row r="39" spans="1:26" ht="15.75" customHeight="1">
-      <c r="A39" s="31" t="s">
+      <c r="A39" s="30" t="s">
         <v>95</v>
       </c>
-      <c r="B39" s="32" t="s">
+      <c r="B39" s="31" t="s">
         <v>85</v>
       </c>
-      <c r="C39" s="33" t="s">
+      <c r="C39" s="32" t="s">
         <v>11</v>
       </c>
-      <c r="D39" s="33" t="s">
+      <c r="D39" s="32" t="s">
         <v>34</v>
       </c>
-      <c r="E39" s="34" t="s">
+      <c r="E39" s="33" t="s">
         <v>96</v>
       </c>
-      <c r="F39" s="35" t="s">
+      <c r="F39" s="34" t="s">
         <v>36</v>
       </c>
-      <c r="G39" s="33"/>
-      <c r="H39" s="33"/>
-      <c r="I39" s="32"/>
-      <c r="J39" s="36"/>
-      <c r="K39" s="36"/>
-      <c r="L39" s="36"/>
-      <c r="M39" s="36"/>
-      <c r="N39" s="36"/>
-      <c r="O39" s="36"/>
-      <c r="P39" s="36"/>
-      <c r="Q39" s="36"/>
-      <c r="R39" s="36"/>
-      <c r="S39" s="36"/>
-      <c r="T39" s="36"/>
-      <c r="U39" s="36"/>
-      <c r="V39" s="36"/>
-      <c r="W39" s="36"/>
-      <c r="X39" s="36"/>
-      <c r="Y39" s="36"/>
-      <c r="Z39" s="36"/>
+      <c r="G39" s="32"/>
+      <c r="H39" s="32"/>
+      <c r="I39" s="31"/>
+      <c r="J39" s="35"/>
+      <c r="K39" s="35"/>
+      <c r="L39" s="35"/>
+      <c r="M39" s="35"/>
+      <c r="N39" s="35"/>
+      <c r="O39" s="35"/>
+      <c r="P39" s="35"/>
+      <c r="Q39" s="35"/>
+      <c r="R39" s="35"/>
+      <c r="S39" s="35"/>
+      <c r="T39" s="35"/>
+      <c r="U39" s="35"/>
+      <c r="V39" s="35"/>
+      <c r="W39" s="35"/>
+      <c r="X39" s="35"/>
+      <c r="Y39" s="35"/>
+      <c r="Z39" s="35"/>
     </row>
     <row r="40" spans="1:26" ht="15.75" customHeight="1">
-      <c r="A40" s="31" t="s">
+      <c r="A40" s="30" t="s">
         <v>97</v>
       </c>
-      <c r="B40" s="32" t="s">
+      <c r="B40" s="31" t="s">
         <v>85</v>
       </c>
-      <c r="C40" s="33" t="s">
+      <c r="C40" s="32" t="s">
         <v>80</v>
       </c>
-      <c r="D40" s="33" t="s">
+      <c r="D40" s="32" t="s">
         <v>34</v>
       </c>
-      <c r="E40" s="34" t="s">
+      <c r="E40" s="33" t="s">
         <v>98</v>
       </c>
-      <c r="F40" s="35" t="s">
+      <c r="F40" s="34" t="s">
         <v>14</v>
       </c>
-      <c r="G40" s="33"/>
-      <c r="H40" s="33"/>
-      <c r="I40" s="32"/>
-      <c r="J40" s="36"/>
-      <c r="K40" s="36"/>
-      <c r="L40" s="36"/>
-      <c r="M40" s="36"/>
-      <c r="N40" s="36"/>
-      <c r="O40" s="36"/>
-      <c r="P40" s="36"/>
-      <c r="Q40" s="36"/>
-      <c r="R40" s="36"/>
-      <c r="S40" s="36"/>
-      <c r="T40" s="36"/>
-      <c r="U40" s="36"/>
-      <c r="V40" s="36"/>
-      <c r="W40" s="36"/>
-      <c r="X40" s="36"/>
-      <c r="Y40" s="36"/>
-      <c r="Z40" s="36"/>
+      <c r="G40" s="32"/>
+      <c r="H40" s="32"/>
+      <c r="I40" s="31"/>
+      <c r="J40" s="35"/>
+      <c r="K40" s="35"/>
+      <c r="L40" s="35"/>
+      <c r="M40" s="35"/>
+      <c r="N40" s="35"/>
+      <c r="O40" s="35"/>
+      <c r="P40" s="35"/>
+      <c r="Q40" s="35"/>
+      <c r="R40" s="35"/>
+      <c r="S40" s="35"/>
+      <c r="T40" s="35"/>
+      <c r="U40" s="35"/>
+      <c r="V40" s="35"/>
+      <c r="W40" s="35"/>
+      <c r="X40" s="35"/>
+      <c r="Y40" s="35"/>
+      <c r="Z40" s="35"/>
     </row>
     <row r="41" spans="1:26" ht="15.75" customHeight="1">
-      <c r="A41" s="31" t="s">
+      <c r="A41" s="30" t="s">
         <v>99</v>
       </c>
-      <c r="B41" s="32" t="s">
+      <c r="B41" s="31" t="s">
         <v>85</v>
       </c>
-      <c r="C41" s="33" t="s">
+      <c r="C41" s="32" t="s">
         <v>80</v>
       </c>
-      <c r="D41" s="33" t="s">
+      <c r="D41" s="32" t="s">
         <v>34</v>
       </c>
-      <c r="E41" s="34" t="s">
+      <c r="E41" s="33" t="s">
         <v>100</v>
       </c>
-      <c r="F41" s="35" t="s">
+      <c r="F41" s="34" t="s">
         <v>14</v>
       </c>
-      <c r="G41" s="33"/>
-      <c r="H41" s="33"/>
-      <c r="I41" s="32"/>
-      <c r="J41" s="36"/>
-      <c r="K41" s="36"/>
-      <c r="L41" s="36"/>
-      <c r="M41" s="36"/>
-      <c r="N41" s="36"/>
-      <c r="O41" s="36"/>
-      <c r="P41" s="36"/>
-      <c r="Q41" s="36"/>
-      <c r="R41" s="36"/>
-      <c r="S41" s="36"/>
-      <c r="T41" s="36"/>
-      <c r="U41" s="36"/>
-      <c r="V41" s="36"/>
-      <c r="W41" s="36"/>
-      <c r="X41" s="36"/>
-      <c r="Y41" s="36"/>
-      <c r="Z41" s="36"/>
+      <c r="G41" s="32"/>
+      <c r="H41" s="32"/>
+      <c r="I41" s="31"/>
+      <c r="J41" s="35"/>
+      <c r="K41" s="35"/>
+      <c r="L41" s="35"/>
+      <c r="M41" s="35"/>
+      <c r="N41" s="35"/>
+      <c r="O41" s="35"/>
+      <c r="P41" s="35"/>
+      <c r="Q41" s="35"/>
+      <c r="R41" s="35"/>
+      <c r="S41" s="35"/>
+      <c r="T41" s="35"/>
+      <c r="U41" s="35"/>
+      <c r="V41" s="35"/>
+      <c r="W41" s="35"/>
+      <c r="X41" s="35"/>
+      <c r="Y41" s="35"/>
+      <c r="Z41" s="35"/>
     </row>
     <row r="42" spans="1:26" ht="15.75" customHeight="1">
-      <c r="A42" s="31" t="s">
+      <c r="A42" s="30" t="s">
         <v>101</v>
       </c>
-      <c r="B42" s="32" t="s">
+      <c r="B42" s="31" t="s">
         <v>85</v>
       </c>
-      <c r="C42" s="37" t="s">
+      <c r="C42" s="36" t="s">
         <v>80</v>
       </c>
-      <c r="D42" s="37" t="s">
+      <c r="D42" s="36" t="s">
         <v>34</v>
       </c>
-      <c r="E42" s="38" t="s">
+      <c r="E42" s="37" t="s">
         <v>102</v>
       </c>
-      <c r="F42" s="39" t="s">
+      <c r="F42" s="38" t="s">
         <v>14</v>
       </c>
-      <c r="G42" s="33"/>
-      <c r="H42" s="37"/>
-      <c r="I42" s="40"/>
-      <c r="J42" s="36"/>
-      <c r="K42" s="36"/>
-      <c r="L42" s="36"/>
-      <c r="M42" s="36"/>
-      <c r="N42" s="36"/>
-      <c r="O42" s="36"/>
-      <c r="P42" s="36"/>
-      <c r="Q42" s="36"/>
-      <c r="R42" s="36"/>
-      <c r="S42" s="36"/>
-      <c r="T42" s="36"/>
-      <c r="U42" s="36"/>
-      <c r="V42" s="36"/>
-      <c r="W42" s="36"/>
-      <c r="X42" s="36"/>
-      <c r="Y42" s="36"/>
-      <c r="Z42" s="36"/>
+      <c r="G42" s="32"/>
+      <c r="H42" s="36"/>
+      <c r="I42" s="39"/>
+      <c r="J42" s="35"/>
+      <c r="K42" s="35"/>
+      <c r="L42" s="35"/>
+      <c r="M42" s="35"/>
+      <c r="N42" s="35"/>
+      <c r="O42" s="35"/>
+      <c r="P42" s="35"/>
+      <c r="Q42" s="35"/>
+      <c r="R42" s="35"/>
+      <c r="S42" s="35"/>
+      <c r="T42" s="35"/>
+      <c r="U42" s="35"/>
+      <c r="V42" s="35"/>
+      <c r="W42" s="35"/>
+      <c r="X42" s="35"/>
+      <c r="Y42" s="35"/>
+      <c r="Z42" s="35"/>
     </row>
     <row r="43" spans="1:26" ht="15.75" customHeight="1">
-      <c r="A43" s="31" t="s">
+      <c r="A43" s="30" t="s">
         <v>103</v>
       </c>
-      <c r="B43" s="32" t="s">
+      <c r="B43" s="31" t="s">
         <v>85</v>
       </c>
-      <c r="C43" s="41" t="s">
+      <c r="C43" s="40" t="s">
         <v>80</v>
       </c>
-      <c r="D43" s="41" t="s">
+      <c r="D43" s="40" t="s">
         <v>34</v>
       </c>
-      <c r="E43" s="42" t="s">
+      <c r="E43" s="41" t="s">
         <v>104</v>
       </c>
-      <c r="F43" s="43" t="s">
+      <c r="F43" s="42" t="s">
         <v>14</v>
       </c>
-      <c r="G43" s="33"/>
-      <c r="H43" s="41"/>
-      <c r="I43" s="44"/>
-      <c r="J43" s="36"/>
-      <c r="K43" s="36"/>
-      <c r="L43" s="36"/>
-      <c r="M43" s="36"/>
-      <c r="N43" s="36"/>
-      <c r="O43" s="36"/>
-      <c r="P43" s="36"/>
-      <c r="Q43" s="36"/>
-      <c r="R43" s="36"/>
-      <c r="S43" s="36"/>
-      <c r="T43" s="36"/>
-      <c r="U43" s="36"/>
-      <c r="V43" s="36"/>
-      <c r="W43" s="36"/>
-      <c r="X43" s="36"/>
-      <c r="Y43" s="36"/>
-      <c r="Z43" s="36"/>
+      <c r="G43" s="32"/>
+      <c r="H43" s="40"/>
+      <c r="I43" s="43"/>
+      <c r="J43" s="35"/>
+      <c r="K43" s="35"/>
+      <c r="L43" s="35"/>
+      <c r="M43" s="35"/>
+      <c r="N43" s="35"/>
+      <c r="O43" s="35"/>
+      <c r="P43" s="35"/>
+      <c r="Q43" s="35"/>
+      <c r="R43" s="35"/>
+      <c r="S43" s="35"/>
+      <c r="T43" s="35"/>
+      <c r="U43" s="35"/>
+      <c r="V43" s="35"/>
+      <c r="W43" s="35"/>
+      <c r="X43" s="35"/>
+      <c r="Y43" s="35"/>
+      <c r="Z43" s="35"/>
     </row>
     <row r="44" spans="1:26" ht="15.75" customHeight="1">
-      <c r="A44" s="31" t="s">
+      <c r="A44" s="30" t="s">
         <v>105</v>
       </c>
-      <c r="B44" s="32" t="s">
+      <c r="B44" s="31" t="s">
         <v>85</v>
       </c>
-      <c r="C44" s="33" t="s">
+      <c r="C44" s="32" t="s">
         <v>80</v>
       </c>
-      <c r="D44" s="33" t="s">
+      <c r="D44" s="32" t="s">
         <v>34</v>
       </c>
-      <c r="E44" s="34" t="s">
+      <c r="E44" s="33" t="s">
         <v>106</v>
       </c>
-      <c r="F44" s="35" t="s">
+      <c r="F44" s="34" t="s">
         <v>21</v>
       </c>
-      <c r="G44" s="33"/>
-      <c r="H44" s="33"/>
-      <c r="I44" s="32"/>
-      <c r="J44" s="36"/>
-      <c r="K44" s="36"/>
-      <c r="L44" s="36"/>
-      <c r="M44" s="36"/>
-      <c r="N44" s="36"/>
-      <c r="O44" s="36"/>
-      <c r="P44" s="36"/>
-      <c r="Q44" s="36"/>
-      <c r="R44" s="36"/>
-      <c r="S44" s="36"/>
-      <c r="T44" s="36"/>
-      <c r="U44" s="36"/>
-      <c r="V44" s="36"/>
-      <c r="W44" s="36"/>
-      <c r="X44" s="36"/>
-      <c r="Y44" s="36"/>
-      <c r="Z44" s="36"/>
+      <c r="G44" s="32"/>
+      <c r="H44" s="32"/>
+      <c r="I44" s="31"/>
+      <c r="J44" s="35"/>
+      <c r="K44" s="35"/>
+      <c r="L44" s="35"/>
+      <c r="M44" s="35"/>
+      <c r="N44" s="35"/>
+      <c r="O44" s="35"/>
+      <c r="P44" s="35"/>
+      <c r="Q44" s="35"/>
+      <c r="R44" s="35"/>
+      <c r="S44" s="35"/>
+      <c r="T44" s="35"/>
+      <c r="U44" s="35"/>
+      <c r="V44" s="35"/>
+      <c r="W44" s="35"/>
+      <c r="X44" s="35"/>
+      <c r="Y44" s="35"/>
+      <c r="Z44" s="35"/>
     </row>
     <row r="45" spans="1:26" ht="15.75" customHeight="1">
-      <c r="A45" s="31" t="s">
+      <c r="A45" s="30" t="s">
         <v>107</v>
       </c>
-      <c r="B45" s="32" t="s">
+      <c r="B45" s="31" t="s">
         <v>85</v>
       </c>
-      <c r="C45" s="33" t="s">
+      <c r="C45" s="32" t="s">
         <v>80</v>
       </c>
-      <c r="D45" s="33" t="s">
+      <c r="D45" s="32" t="s">
         <v>34</v>
       </c>
-      <c r="E45" s="34" t="s">
+      <c r="E45" s="33" t="s">
         <v>108</v>
       </c>
-      <c r="F45" s="35" t="s">
+      <c r="F45" s="34" t="s">
         <v>21</v>
       </c>
-      <c r="G45" s="33"/>
-      <c r="H45" s="33"/>
-      <c r="I45" s="32"/>
-      <c r="J45" s="36"/>
-      <c r="K45" s="36"/>
-      <c r="L45" s="36"/>
-      <c r="M45" s="36"/>
-      <c r="N45" s="36"/>
-      <c r="O45" s="36"/>
-      <c r="P45" s="36"/>
-      <c r="Q45" s="36"/>
-      <c r="R45" s="36"/>
-      <c r="S45" s="36"/>
-      <c r="T45" s="36"/>
-      <c r="U45" s="36"/>
-      <c r="V45" s="36"/>
-      <c r="W45" s="36"/>
-      <c r="X45" s="36"/>
-      <c r="Y45" s="36"/>
-      <c r="Z45" s="36"/>
+      <c r="G45" s="32"/>
+      <c r="H45" s="32"/>
+      <c r="I45" s="31"/>
+      <c r="J45" s="35"/>
+      <c r="K45" s="35"/>
+      <c r="L45" s="35"/>
+      <c r="M45" s="35"/>
+      <c r="N45" s="35"/>
+      <c r="O45" s="35"/>
+      <c r="P45" s="35"/>
+      <c r="Q45" s="35"/>
+      <c r="R45" s="35"/>
+      <c r="S45" s="35"/>
+      <c r="T45" s="35"/>
+      <c r="U45" s="35"/>
+      <c r="V45" s="35"/>
+      <c r="W45" s="35"/>
+      <c r="X45" s="35"/>
+      <c r="Y45" s="35"/>
+      <c r="Z45" s="35"/>
     </row>
     <row r="46" spans="1:26" ht="15.75" customHeight="1">
-      <c r="A46" s="31" t="s">
+      <c r="A46" s="30" t="s">
         <v>109</v>
       </c>
-      <c r="B46" s="32" t="s">
+      <c r="B46" s="31" t="s">
         <v>85</v>
       </c>
-      <c r="C46" s="33" t="s">
+      <c r="C46" s="32" t="s">
         <v>80</v>
       </c>
-      <c r="D46" s="33" t="s">
+      <c r="D46" s="32" t="s">
         <v>34</v>
       </c>
-      <c r="E46" s="34" t="s">
+      <c r="E46" s="33" t="s">
         <v>110</v>
       </c>
-      <c r="F46" s="35" t="s">
+      <c r="F46" s="34" t="s">
         <v>21</v>
       </c>
-      <c r="G46" s="33"/>
-      <c r="H46" s="33"/>
-      <c r="I46" s="32"/>
-      <c r="J46" s="36"/>
-      <c r="K46" s="36"/>
-      <c r="L46" s="36"/>
-      <c r="M46" s="36"/>
-      <c r="N46" s="36"/>
-      <c r="O46" s="36"/>
-      <c r="P46" s="36"/>
-      <c r="Q46" s="36"/>
-      <c r="R46" s="36"/>
-      <c r="S46" s="36"/>
-      <c r="T46" s="36"/>
-      <c r="U46" s="36"/>
-      <c r="V46" s="36"/>
-      <c r="W46" s="36"/>
-      <c r="X46" s="36"/>
-      <c r="Y46" s="36"/>
-      <c r="Z46" s="36"/>
+      <c r="G46" s="32"/>
+      <c r="H46" s="32"/>
+      <c r="I46" s="31"/>
+      <c r="J46" s="35"/>
+      <c r="K46" s="35"/>
+      <c r="L46" s="35"/>
+      <c r="M46" s="35"/>
+      <c r="N46" s="35"/>
+      <c r="O46" s="35"/>
+      <c r="P46" s="35"/>
+      <c r="Q46" s="35"/>
+      <c r="R46" s="35"/>
+      <c r="S46" s="35"/>
+      <c r="T46" s="35"/>
+      <c r="U46" s="35"/>
+      <c r="V46" s="35"/>
+      <c r="W46" s="35"/>
+      <c r="X46" s="35"/>
+      <c r="Y46" s="35"/>
+      <c r="Z46" s="35"/>
     </row>
     <row r="47" spans="1:26" ht="15.75" customHeight="1">
-      <c r="A47" s="31" t="s">
+      <c r="A47" s="30" t="s">
         <v>111</v>
       </c>
-      <c r="B47" s="32" t="s">
+      <c r="B47" s="31" t="s">
         <v>85</v>
       </c>
-      <c r="C47" s="33" t="s">
+      <c r="C47" s="32" t="s">
         <v>80</v>
       </c>
-      <c r="D47" s="33" t="s">
+      <c r="D47" s="32" t="s">
         <v>34</v>
       </c>
-      <c r="E47" s="34" t="s">
+      <c r="E47" s="33" t="s">
         <v>112</v>
       </c>
-      <c r="F47" s="35" t="s">
+      <c r="F47" s="34" t="s">
         <v>21</v>
       </c>
-      <c r="G47" s="33"/>
-      <c r="H47" s="33"/>
-      <c r="I47" s="32"/>
-      <c r="J47" s="36"/>
-      <c r="K47" s="36"/>
-      <c r="L47" s="36"/>
-      <c r="M47" s="36"/>
-      <c r="N47" s="36"/>
-      <c r="O47" s="36"/>
-      <c r="P47" s="36"/>
-      <c r="Q47" s="36"/>
-      <c r="R47" s="36"/>
-      <c r="S47" s="36"/>
-      <c r="T47" s="36"/>
-      <c r="U47" s="36"/>
-      <c r="V47" s="36"/>
-      <c r="W47" s="36"/>
-      <c r="X47" s="36"/>
-      <c r="Y47" s="36"/>
-      <c r="Z47" s="36"/>
+      <c r="G47" s="32"/>
+      <c r="H47" s="32"/>
+      <c r="I47" s="31"/>
+      <c r="J47" s="35"/>
+      <c r="K47" s="35"/>
+      <c r="L47" s="35"/>
+      <c r="M47" s="35"/>
+      <c r="N47" s="35"/>
+      <c r="O47" s="35"/>
+      <c r="P47" s="35"/>
+      <c r="Q47" s="35"/>
+      <c r="R47" s="35"/>
+      <c r="S47" s="35"/>
+      <c r="T47" s="35"/>
+      <c r="U47" s="35"/>
+      <c r="V47" s="35"/>
+      <c r="W47" s="35"/>
+      <c r="X47" s="35"/>
+      <c r="Y47" s="35"/>
+      <c r="Z47" s="35"/>
     </row>
     <row r="48" spans="1:26" ht="15.75" customHeight="1">
-      <c r="A48" s="31" t="s">
+      <c r="A48" s="30" t="s">
         <v>113</v>
       </c>
-      <c r="B48" s="32" t="s">
+      <c r="B48" s="31" t="s">
         <v>85</v>
       </c>
-      <c r="C48" s="33" t="s">
+      <c r="C48" s="32" t="s">
         <v>55</v>
       </c>
-      <c r="D48" s="33" t="s">
+      <c r="D48" s="32" t="s">
         <v>34</v>
       </c>
-      <c r="E48" s="34" t="s">
+      <c r="E48" s="33" t="s">
         <v>114</v>
       </c>
-      <c r="F48" s="35" t="s">
+      <c r="F48" s="34" t="s">
         <v>14</v>
       </c>
-      <c r="G48" s="33"/>
-      <c r="H48" s="33"/>
-      <c r="I48" s="32"/>
-      <c r="J48" s="36"/>
-      <c r="K48" s="36"/>
-      <c r="L48" s="36"/>
-      <c r="M48" s="36"/>
-      <c r="N48" s="36"/>
-      <c r="O48" s="36"/>
-      <c r="P48" s="36"/>
-      <c r="Q48" s="36"/>
-      <c r="R48" s="36"/>
-      <c r="S48" s="36"/>
-      <c r="T48" s="36"/>
-      <c r="U48" s="36"/>
-      <c r="V48" s="36"/>
-      <c r="W48" s="36"/>
-      <c r="X48" s="36"/>
-      <c r="Y48" s="36"/>
-      <c r="Z48" s="36"/>
+      <c r="G48" s="32"/>
+      <c r="H48" s="32"/>
+      <c r="I48" s="31"/>
+      <c r="J48" s="35"/>
+      <c r="K48" s="35"/>
+      <c r="L48" s="35"/>
+      <c r="M48" s="35"/>
+      <c r="N48" s="35"/>
+      <c r="O48" s="35"/>
+      <c r="P48" s="35"/>
+      <c r="Q48" s="35"/>
+      <c r="R48" s="35"/>
+      <c r="S48" s="35"/>
+      <c r="T48" s="35"/>
+      <c r="U48" s="35"/>
+      <c r="V48" s="35"/>
+      <c r="W48" s="35"/>
+      <c r="X48" s="35"/>
+      <c r="Y48" s="35"/>
+      <c r="Z48" s="35"/>
     </row>
     <row r="49" spans="1:26" ht="15.75" customHeight="1">
-      <c r="A49" s="31" t="s">
+      <c r="A49" s="30" t="s">
         <v>115</v>
       </c>
-      <c r="B49" s="32" t="s">
+      <c r="B49" s="31" t="s">
         <v>85</v>
       </c>
-      <c r="C49" s="33" t="s">
+      <c r="C49" s="32" t="s">
         <v>55</v>
       </c>
-      <c r="D49" s="33" t="s">
+      <c r="D49" s="32" t="s">
         <v>34</v>
       </c>
-      <c r="E49" s="34" t="s">
+      <c r="E49" s="33" t="s">
         <v>116</v>
       </c>
-      <c r="F49" s="35" t="s">
+      <c r="F49" s="34" t="s">
         <v>36</v>
       </c>
-      <c r="G49" s="33"/>
-      <c r="H49" s="33"/>
-      <c r="I49" s="32"/>
-      <c r="J49" s="36"/>
-      <c r="K49" s="36"/>
-      <c r="L49" s="36"/>
-      <c r="M49" s="36"/>
-      <c r="N49" s="36"/>
-      <c r="O49" s="36"/>
-      <c r="P49" s="36"/>
-      <c r="Q49" s="36"/>
-      <c r="R49" s="36"/>
-      <c r="S49" s="36"/>
-      <c r="T49" s="36"/>
-      <c r="U49" s="36"/>
-      <c r="V49" s="36"/>
-      <c r="W49" s="36"/>
-      <c r="X49" s="36"/>
-      <c r="Y49" s="36"/>
-      <c r="Z49" s="36"/>
+      <c r="G49" s="32"/>
+      <c r="H49" s="32"/>
+      <c r="I49" s="31"/>
+      <c r="J49" s="35"/>
+      <c r="K49" s="35"/>
+      <c r="L49" s="35"/>
+      <c r="M49" s="35"/>
+      <c r="N49" s="35"/>
+      <c r="O49" s="35"/>
+      <c r="P49" s="35"/>
+      <c r="Q49" s="35"/>
+      <c r="R49" s="35"/>
+      <c r="S49" s="35"/>
+      <c r="T49" s="35"/>
+      <c r="U49" s="35"/>
+      <c r="V49" s="35"/>
+      <c r="W49" s="35"/>
+      <c r="X49" s="35"/>
+      <c r="Y49" s="35"/>
+      <c r="Z49" s="35"/>
     </row>
     <row r="50" spans="1:26" ht="15.75" customHeight="1">
-      <c r="A50" s="31" t="s">
+      <c r="A50" s="30" t="s">
         <v>117</v>
       </c>
-      <c r="B50" s="32" t="s">
+      <c r="B50" s="31" t="s">
         <v>85</v>
       </c>
-      <c r="C50" s="33" t="s">
+      <c r="C50" s="32" t="s">
         <v>55</v>
       </c>
-      <c r="D50" s="33" t="s">
+      <c r="D50" s="32" t="s">
         <v>34</v>
       </c>
-      <c r="E50" s="34" t="s">
+      <c r="E50" s="33" t="s">
         <v>118</v>
       </c>
-      <c r="F50" s="35" t="s">
+      <c r="F50" s="34" t="s">
         <v>21</v>
       </c>
-      <c r="G50" s="33"/>
-      <c r="H50" s="33"/>
-      <c r="I50" s="32"/>
-      <c r="J50" s="36"/>
-      <c r="K50" s="36"/>
-      <c r="L50" s="36"/>
-      <c r="M50" s="36"/>
-      <c r="N50" s="36"/>
-      <c r="O50" s="36"/>
-      <c r="P50" s="36"/>
-      <c r="Q50" s="36"/>
-      <c r="R50" s="36"/>
-      <c r="S50" s="36"/>
-      <c r="T50" s="36"/>
-      <c r="U50" s="36"/>
-      <c r="V50" s="36"/>
-      <c r="W50" s="36"/>
-      <c r="X50" s="36"/>
-      <c r="Y50" s="36"/>
-      <c r="Z50" s="36"/>
+      <c r="G50" s="32"/>
+      <c r="H50" s="32"/>
+      <c r="I50" s="31"/>
+      <c r="J50" s="35"/>
+      <c r="K50" s="35"/>
+      <c r="L50" s="35"/>
+      <c r="M50" s="35"/>
+      <c r="N50" s="35"/>
+      <c r="O50" s="35"/>
+      <c r="P50" s="35"/>
+      <c r="Q50" s="35"/>
+      <c r="R50" s="35"/>
+      <c r="S50" s="35"/>
+      <c r="T50" s="35"/>
+      <c r="U50" s="35"/>
+      <c r="V50" s="35"/>
+      <c r="W50" s="35"/>
+      <c r="X50" s="35"/>
+      <c r="Y50" s="35"/>
+      <c r="Z50" s="35"/>
     </row>
     <row r="51" spans="1:26" ht="15.75" customHeight="1">
-      <c r="A51" s="31" t="s">
+      <c r="A51" s="30" t="s">
         <v>119</v>
       </c>
-      <c r="B51" s="32" t="s">
+      <c r="B51" s="31" t="s">
         <v>85</v>
       </c>
-      <c r="C51" s="33" t="s">
+      <c r="C51" s="32" t="s">
         <v>55</v>
       </c>
-      <c r="D51" s="33" t="s">
+      <c r="D51" s="32" t="s">
         <v>34</v>
       </c>
-      <c r="E51" s="34" t="s">
+      <c r="E51" s="33" t="s">
         <v>120</v>
       </c>
-      <c r="F51" s="35" t="s">
+      <c r="F51" s="34" t="s">
         <v>14</v>
       </c>
-      <c r="G51" s="33"/>
-      <c r="H51" s="33"/>
-      <c r="I51" s="32"/>
-      <c r="J51" s="36"/>
-      <c r="K51" s="36"/>
-      <c r="L51" s="36"/>
-      <c r="M51" s="36"/>
-      <c r="N51" s="36"/>
-      <c r="O51" s="36"/>
-      <c r="P51" s="36"/>
-      <c r="Q51" s="36"/>
-      <c r="R51" s="36"/>
-      <c r="S51" s="36"/>
-      <c r="T51" s="36"/>
-      <c r="U51" s="36"/>
-      <c r="V51" s="36"/>
-      <c r="W51" s="36"/>
-      <c r="X51" s="36"/>
-      <c r="Y51" s="36"/>
-      <c r="Z51" s="36"/>
+      <c r="G51" s="32"/>
+      <c r="H51" s="32"/>
+      <c r="I51" s="31"/>
+      <c r="J51" s="35"/>
+      <c r="K51" s="35"/>
+      <c r="L51" s="35"/>
+      <c r="M51" s="35"/>
+      <c r="N51" s="35"/>
+      <c r="O51" s="35"/>
+      <c r="P51" s="35"/>
+      <c r="Q51" s="35"/>
+      <c r="R51" s="35"/>
+      <c r="S51" s="35"/>
+      <c r="T51" s="35"/>
+      <c r="U51" s="35"/>
+      <c r="V51" s="35"/>
+      <c r="W51" s="35"/>
+      <c r="X51" s="35"/>
+      <c r="Y51" s="35"/>
+      <c r="Z51" s="35"/>
     </row>
     <row r="52" spans="1:26" ht="15.75" customHeight="1">
-      <c r="A52" s="31" t="s">
+      <c r="A52" s="30" t="s">
         <v>121</v>
       </c>
-      <c r="B52" s="32" t="s">
+      <c r="B52" s="31" t="s">
         <v>85</v>
       </c>
-      <c r="C52" s="33" t="s">
+      <c r="C52" s="32" t="s">
         <v>55</v>
       </c>
-      <c r="D52" s="33" t="s">
+      <c r="D52" s="32" t="s">
         <v>34</v>
       </c>
-      <c r="E52" s="34" t="s">
+      <c r="E52" s="33" t="s">
         <v>122</v>
       </c>
-      <c r="F52" s="35" t="s">
+      <c r="F52" s="34" t="s">
         <v>21</v>
       </c>
-      <c r="G52" s="33"/>
-      <c r="H52" s="33"/>
-      <c r="I52" s="32"/>
-      <c r="J52" s="36"/>
-      <c r="K52" s="36"/>
-      <c r="L52" s="36"/>
-      <c r="M52" s="36"/>
-      <c r="N52" s="36"/>
-      <c r="O52" s="36"/>
-      <c r="P52" s="36"/>
-      <c r="Q52" s="36"/>
-      <c r="R52" s="36"/>
-      <c r="S52" s="36"/>
-      <c r="T52" s="36"/>
-      <c r="U52" s="36"/>
-      <c r="V52" s="36"/>
-      <c r="W52" s="36"/>
-      <c r="X52" s="36"/>
-      <c r="Y52" s="36"/>
-      <c r="Z52" s="36"/>
+      <c r="G52" s="32"/>
+      <c r="H52" s="32"/>
+      <c r="I52" s="31"/>
+      <c r="J52" s="35"/>
+      <c r="K52" s="35"/>
+      <c r="L52" s="35"/>
+      <c r="M52" s="35"/>
+      <c r="N52" s="35"/>
+      <c r="O52" s="35"/>
+      <c r="P52" s="35"/>
+      <c r="Q52" s="35"/>
+      <c r="R52" s="35"/>
+      <c r="S52" s="35"/>
+      <c r="T52" s="35"/>
+      <c r="U52" s="35"/>
+      <c r="V52" s="35"/>
+      <c r="W52" s="35"/>
+      <c r="X52" s="35"/>
+      <c r="Y52" s="35"/>
+      <c r="Z52" s="35"/>
     </row>
     <row r="53" spans="1:26" ht="15.75" customHeight="1">
       <c r="A53" s="21" t="s">
@@ -3545,27 +3545,27 @@
       <c r="Z56" s="20"/>
     </row>
     <row r="57" spans="1:26" ht="15.75" customHeight="1">
-      <c r="A57" s="24" t="s">
+      <c r="A57" s="23" t="s">
         <v>132</v>
       </c>
-      <c r="B57" s="25" t="s">
+      <c r="B57" s="24" t="s">
         <v>124</v>
       </c>
-      <c r="C57" s="26" t="s">
+      <c r="C57" s="25" t="s">
         <v>55</v>
       </c>
-      <c r="D57" s="26" t="s">
+      <c r="D57" s="25" t="s">
         <v>34</v>
       </c>
-      <c r="E57" s="25" t="s">
+      <c r="E57" s="24" t="s">
         <v>133</v>
       </c>
-      <c r="F57" s="25" t="s">
+      <c r="F57" s="24" t="s">
         <v>21</v>
       </c>
-      <c r="G57" s="26"/>
-      <c r="H57" s="26"/>
-      <c r="I57" s="25"/>
+      <c r="G57" s="25"/>
+      <c r="H57" s="25"/>
+      <c r="I57" s="24"/>
       <c r="J57" s="20"/>
       <c r="K57" s="20"/>
       <c r="L57" s="20"/>
@@ -3585,27 +3585,27 @@
       <c r="Z57" s="20"/>
     </row>
     <row r="58" spans="1:26" ht="15.75" customHeight="1">
-      <c r="A58" s="28" t="s">
+      <c r="A58" s="27" t="s">
         <v>134</v>
       </c>
-      <c r="B58" s="29" t="s">
+      <c r="B58" s="28" t="s">
         <v>124</v>
       </c>
-      <c r="C58" s="30" t="s">
+      <c r="C58" s="29" t="s">
         <v>80</v>
       </c>
-      <c r="D58" s="30" t="s">
+      <c r="D58" s="29" t="s">
         <v>34</v>
       </c>
-      <c r="E58" s="29" t="s">
+      <c r="E58" s="28" t="s">
         <v>135</v>
       </c>
-      <c r="F58" s="29" t="s">
+      <c r="F58" s="28" t="s">
         <v>36</v>
       </c>
-      <c r="G58" s="30"/>
-      <c r="H58" s="30"/>
-      <c r="I58" s="29"/>
+      <c r="G58" s="29"/>
+      <c r="H58" s="29"/>
+      <c r="I58" s="28"/>
       <c r="J58" s="20"/>
       <c r="K58" s="20"/>
       <c r="L58" s="20"/>
@@ -3640,7 +3640,7 @@
       <c r="E59" s="18" t="s">
         <v>138</v>
       </c>
-      <c r="F59" s="45" t="s">
+      <c r="F59" s="44" t="s">
         <v>14</v>
       </c>
       <c r="G59" s="19"/>
@@ -3680,7 +3680,7 @@
       <c r="E60" s="18" t="s">
         <v>140</v>
       </c>
-      <c r="F60" s="45" t="s">
+      <c r="F60" s="44" t="s">
         <v>14</v>
       </c>
       <c r="G60" s="19"/>
@@ -3720,7 +3720,7 @@
       <c r="E61" s="18" t="s">
         <v>142</v>
       </c>
-      <c r="F61" s="45" t="s">
+      <c r="F61" s="44" t="s">
         <v>14</v>
       </c>
       <c r="G61" s="19"/>
@@ -3760,7 +3760,7 @@
       <c r="E62" s="18" t="s">
         <v>144</v>
       </c>
-      <c r="F62" s="45" t="s">
+      <c r="F62" s="44" t="s">
         <v>21</v>
       </c>
       <c r="G62" s="19"/>
@@ -3800,7 +3800,7 @@
       <c r="E63" s="18" t="s">
         <v>146</v>
       </c>
-      <c r="F63" s="45" t="s">
+      <c r="F63" s="44" t="s">
         <v>21</v>
       </c>
       <c r="G63" s="19"/>
@@ -3840,7 +3840,7 @@
       <c r="E64" s="18" t="s">
         <v>148</v>
       </c>
-      <c r="F64" s="45" t="s">
+      <c r="F64" s="44" t="s">
         <v>21</v>
       </c>
       <c r="G64" s="19"/>
@@ -3880,7 +3880,7 @@
       <c r="E65" s="18" t="s">
         <v>150</v>
       </c>
-      <c r="F65" s="45" t="s">
+      <c r="F65" s="44" t="s">
         <v>21</v>
       </c>
       <c r="G65" s="19"/>
@@ -3920,7 +3920,7 @@
       <c r="E66" s="18" t="s">
         <v>152</v>
       </c>
-      <c r="F66" s="45" t="s">
+      <c r="F66" s="44" t="s">
         <v>36</v>
       </c>
       <c r="G66" s="19"/>
@@ -3960,7 +3960,7 @@
       <c r="E67" s="18" t="s">
         <v>154</v>
       </c>
-      <c r="F67" s="45" t="s">
+      <c r="F67" s="44" t="s">
         <v>36</v>
       </c>
       <c r="G67" s="19"/>
@@ -3997,10 +3997,10 @@
       <c r="D68" s="19" t="s">
         <v>34</v>
       </c>
-      <c r="E68" s="46" t="s">
+      <c r="E68" s="45" t="s">
         <v>156</v>
       </c>
-      <c r="F68" s="45" t="s">
+      <c r="F68" s="44" t="s">
         <v>14</v>
       </c>
       <c r="G68" s="19"/>
@@ -4025,27 +4025,27 @@
       <c r="Z68" s="20"/>
     </row>
     <row r="69" spans="1:26" ht="15.75" customHeight="1">
-      <c r="A69" s="47" t="s">
+      <c r="A69" s="46" t="s">
         <v>157</v>
       </c>
-      <c r="B69" s="46" t="s">
+      <c r="B69" s="45" t="s">
         <v>137</v>
       </c>
-      <c r="C69" s="48" t="s">
+      <c r="C69" s="47" t="s">
         <v>55</v>
       </c>
-      <c r="D69" s="49" t="s">
+      <c r="D69" s="48" t="s">
         <v>34</v>
       </c>
       <c r="E69" s="18" t="s">
         <v>158</v>
       </c>
-      <c r="F69" s="50" t="s">
+      <c r="F69" s="49" t="s">
         <v>14</v>
       </c>
-      <c r="G69" s="47"/>
-      <c r="H69" s="47"/>
-      <c r="I69" s="46"/>
+      <c r="G69" s="46"/>
+      <c r="H69" s="46"/>
+      <c r="I69" s="45"/>
       <c r="J69" s="20"/>
       <c r="K69" s="20"/>
       <c r="L69" s="20"/>
@@ -4074,7 +4074,7 @@
       <c r="C70" s="19" t="s">
         <v>11</v>
       </c>
-      <c r="D70" s="51" t="s">
+      <c r="D70" s="50" t="s">
         <v>34</v>
       </c>
       <c r="E70" s="18" t="s">
@@ -4083,8 +4083,8 @@
       <c r="F70" s="18" t="s">
         <v>14</v>
       </c>
-      <c r="G70" s="52"/>
-      <c r="H70" s="52"/>
+      <c r="G70" s="51"/>
+      <c r="H70" s="51"/>
       <c r="I70" s="18"/>
       <c r="J70" s="20"/>
       <c r="K70" s="20"/>
@@ -4114,7 +4114,7 @@
       <c r="C71" s="19" t="s">
         <v>11</v>
       </c>
-      <c r="D71" s="51" t="s">
+      <c r="D71" s="50" t="s">
         <v>34</v>
       </c>
       <c r="E71" s="18" t="s">
@@ -4124,8 +4124,8 @@
         <v>21</v>
       </c>
       <c r="G71" s="19"/>
-      <c r="H71" s="52"/>
-      <c r="I71" s="52"/>
+      <c r="H71" s="51"/>
+      <c r="I71" s="51"/>
       <c r="J71" s="20"/>
       <c r="K71" s="20"/>
       <c r="L71" s="20"/>
@@ -4154,7 +4154,7 @@
       <c r="C72" s="19" t="s">
         <v>11</v>
       </c>
-      <c r="D72" s="51" t="s">
+      <c r="D72" s="50" t="s">
         <v>34</v>
       </c>
       <c r="E72" s="18" t="s">
@@ -4164,8 +4164,8 @@
         <v>21</v>
       </c>
       <c r="G72" s="19"/>
-      <c r="H72" s="52"/>
-      <c r="I72" s="52"/>
+      <c r="H72" s="51"/>
+      <c r="I72" s="51"/>
       <c r="J72" s="20"/>
       <c r="K72" s="20"/>
       <c r="L72" s="20"/>
@@ -4194,7 +4194,7 @@
       <c r="C73" s="19" t="s">
         <v>11</v>
       </c>
-      <c r="D73" s="51" t="s">
+      <c r="D73" s="50" t="s">
         <v>34</v>
       </c>
       <c r="E73" s="18" t="s">
@@ -4204,8 +4204,8 @@
         <v>21</v>
       </c>
       <c r="G73" s="19"/>
-      <c r="H73" s="52"/>
-      <c r="I73" s="52"/>
+      <c r="H73" s="51"/>
+      <c r="I73" s="51"/>
       <c r="J73" s="20"/>
       <c r="K73" s="20"/>
       <c r="L73" s="20"/>
@@ -4234,7 +4234,7 @@
       <c r="C74" s="19" t="s">
         <v>11</v>
       </c>
-      <c r="D74" s="51" t="s">
+      <c r="D74" s="50" t="s">
         <v>34</v>
       </c>
       <c r="E74" s="18" t="s">
@@ -4244,8 +4244,8 @@
         <v>14</v>
       </c>
       <c r="G74" s="19"/>
-      <c r="H74" s="52"/>
-      <c r="I74" s="52"/>
+      <c r="H74" s="51"/>
+      <c r="I74" s="51"/>
       <c r="J74" s="20"/>
       <c r="K74" s="20"/>
       <c r="L74" s="20"/>
@@ -4274,7 +4274,7 @@
       <c r="C75" s="19" t="s">
         <v>55</v>
       </c>
-      <c r="D75" s="51" t="s">
+      <c r="D75" s="50" t="s">
         <v>34</v>
       </c>
       <c r="E75" s="18" t="s">
@@ -4284,8 +4284,8 @@
         <v>14</v>
       </c>
       <c r="G75" s="19"/>
-      <c r="H75" s="52"/>
-      <c r="I75" s="52"/>
+      <c r="H75" s="51"/>
+      <c r="I75" s="51"/>
       <c r="J75" s="20"/>
       <c r="K75" s="20"/>
       <c r="L75" s="20"/>
@@ -4314,7 +4314,7 @@
       <c r="C76" s="19" t="s">
         <v>55</v>
       </c>
-      <c r="D76" s="51" t="s">
+      <c r="D76" s="50" t="s">
         <v>34</v>
       </c>
       <c r="E76" s="18" t="s">
@@ -4324,8 +4324,8 @@
         <v>14</v>
       </c>
       <c r="G76" s="19"/>
-      <c r="H76" s="52"/>
-      <c r="I76" s="52"/>
+      <c r="H76" s="51"/>
+      <c r="I76" s="51"/>
       <c r="J76" s="20"/>
       <c r="K76" s="20"/>
       <c r="L76" s="20"/>
@@ -4345,571 +4345,571 @@
       <c r="Z76" s="20"/>
     </row>
     <row r="77" spans="1:26" ht="15.75" customHeight="1">
-      <c r="A77" s="36"/>
+      <c r="A77" s="35"/>
     </row>
     <row r="78" spans="1:26" ht="15.75" customHeight="1"/>
     <row r="79" spans="1:26" ht="15.75" customHeight="1"/>
     <row r="80" spans="1:26" ht="15.75" customHeight="1"/>
     <row r="81" spans="1:1" ht="15.75" customHeight="1">
-      <c r="A81" s="36"/>
+      <c r="A81" s="35"/>
     </row>
     <row r="82" spans="1:1" ht="15.75" customHeight="1">
-      <c r="A82" s="36"/>
+      <c r="A82" s="35"/>
     </row>
     <row r="83" spans="1:1" ht="15.75" customHeight="1">
-      <c r="A83" s="36"/>
+      <c r="A83" s="35"/>
     </row>
     <row r="84" spans="1:1" ht="15.75" customHeight="1">
-      <c r="A84" s="36"/>
+      <c r="A84" s="35"/>
     </row>
     <row r="85" spans="1:1" ht="15.75" customHeight="1">
-      <c r="A85" s="36"/>
+      <c r="A85" s="35"/>
     </row>
     <row r="86" spans="1:1" ht="15.75" customHeight="1">
-      <c r="A86" s="36"/>
+      <c r="A86" s="35"/>
     </row>
     <row r="87" spans="1:1" ht="15.75" customHeight="1">
-      <c r="A87" s="36"/>
+      <c r="A87" s="35"/>
     </row>
     <row r="88" spans="1:1" ht="15.75" customHeight="1">
-      <c r="A88" s="36"/>
+      <c r="A88" s="35"/>
     </row>
     <row r="89" spans="1:1" ht="15.75" customHeight="1">
-      <c r="A89" s="36"/>
+      <c r="A89" s="35"/>
     </row>
     <row r="90" spans="1:1" ht="15.75" customHeight="1">
-      <c r="A90" s="36"/>
+      <c r="A90" s="35"/>
     </row>
     <row r="91" spans="1:1" ht="15.75" customHeight="1">
-      <c r="A91" s="36"/>
+      <c r="A91" s="35"/>
     </row>
     <row r="92" spans="1:1" ht="15.75" customHeight="1">
-      <c r="A92" s="36"/>
+      <c r="A92" s="35"/>
     </row>
     <row r="93" spans="1:1" ht="15.75" customHeight="1">
-      <c r="A93" s="36"/>
+      <c r="A93" s="35"/>
     </row>
     <row r="94" spans="1:1" ht="15.75" customHeight="1">
-      <c r="A94" s="36"/>
+      <c r="A94" s="35"/>
     </row>
     <row r="95" spans="1:1" ht="15.75" customHeight="1">
-      <c r="A95" s="36"/>
+      <c r="A95" s="35"/>
     </row>
     <row r="96" spans="1:1" ht="15.75" customHeight="1">
-      <c r="A96" s="36"/>
+      <c r="A96" s="35"/>
     </row>
     <row r="97" spans="1:1" ht="15.75" customHeight="1">
-      <c r="A97" s="36"/>
+      <c r="A97" s="35"/>
     </row>
     <row r="98" spans="1:1" ht="15.75" customHeight="1">
-      <c r="A98" s="36"/>
+      <c r="A98" s="35"/>
     </row>
     <row r="99" spans="1:1" ht="15.75" customHeight="1">
-      <c r="A99" s="36"/>
+      <c r="A99" s="35"/>
     </row>
     <row r="100" spans="1:1" ht="15.75" customHeight="1">
-      <c r="A100" s="36"/>
+      <c r="A100" s="35"/>
     </row>
     <row r="101" spans="1:1" ht="15.75" customHeight="1">
-      <c r="A101" s="36"/>
+      <c r="A101" s="35"/>
     </row>
     <row r="102" spans="1:1" ht="15.75" customHeight="1">
-      <c r="A102" s="36"/>
+      <c r="A102" s="35"/>
     </row>
     <row r="103" spans="1:1" ht="15.75" customHeight="1">
-      <c r="A103" s="36"/>
+      <c r="A103" s="35"/>
     </row>
     <row r="104" spans="1:1" ht="15.75" customHeight="1">
-      <c r="A104" s="36"/>
+      <c r="A104" s="35"/>
     </row>
     <row r="105" spans="1:1" ht="15.75" customHeight="1">
-      <c r="A105" s="36"/>
+      <c r="A105" s="35"/>
     </row>
     <row r="106" spans="1:1" ht="15.75" customHeight="1">
-      <c r="A106" s="36"/>
+      <c r="A106" s="35"/>
     </row>
     <row r="107" spans="1:1" ht="15.75" customHeight="1">
-      <c r="A107" s="36"/>
+      <c r="A107" s="35"/>
     </row>
     <row r="108" spans="1:1" ht="15.75" customHeight="1">
-      <c r="A108" s="36"/>
+      <c r="A108" s="35"/>
     </row>
     <row r="109" spans="1:1" ht="15.75" customHeight="1">
-      <c r="A109" s="36"/>
+      <c r="A109" s="35"/>
     </row>
     <row r="110" spans="1:1" ht="15.75" customHeight="1">
-      <c r="A110" s="36"/>
+      <c r="A110" s="35"/>
     </row>
     <row r="111" spans="1:1" ht="15.75" customHeight="1">
-      <c r="A111" s="36"/>
+      <c r="A111" s="35"/>
     </row>
     <row r="112" spans="1:1" ht="15.75" customHeight="1">
-      <c r="A112" s="36"/>
+      <c r="A112" s="35"/>
     </row>
     <row r="113" spans="1:1" ht="15.75" customHeight="1">
-      <c r="A113" s="36"/>
+      <c r="A113" s="35"/>
     </row>
     <row r="114" spans="1:1" ht="15.75" customHeight="1">
-      <c r="A114" s="36"/>
+      <c r="A114" s="35"/>
     </row>
     <row r="115" spans="1:1" ht="15.75" customHeight="1">
-      <c r="A115" s="36"/>
+      <c r="A115" s="35"/>
     </row>
     <row r="116" spans="1:1" ht="15.75" customHeight="1">
-      <c r="A116" s="36"/>
+      <c r="A116" s="35"/>
     </row>
     <row r="117" spans="1:1" ht="15.75" customHeight="1">
-      <c r="A117" s="36"/>
+      <c r="A117" s="35"/>
     </row>
     <row r="118" spans="1:1" ht="15.75" customHeight="1">
-      <c r="A118" s="36"/>
+      <c r="A118" s="35"/>
     </row>
     <row r="119" spans="1:1" ht="15.75" customHeight="1">
-      <c r="A119" s="36"/>
+      <c r="A119" s="35"/>
     </row>
     <row r="120" spans="1:1" ht="15.75" customHeight="1">
-      <c r="A120" s="36"/>
+      <c r="A120" s="35"/>
     </row>
     <row r="121" spans="1:1" ht="15.75" customHeight="1">
-      <c r="A121" s="36"/>
+      <c r="A121" s="35"/>
     </row>
     <row r="122" spans="1:1" ht="15.75" customHeight="1">
-      <c r="A122" s="36"/>
+      <c r="A122" s="35"/>
     </row>
     <row r="123" spans="1:1" ht="15.75" customHeight="1">
-      <c r="A123" s="36"/>
+      <c r="A123" s="35"/>
     </row>
     <row r="124" spans="1:1" ht="15.75" customHeight="1">
-      <c r="A124" s="36"/>
+      <c r="A124" s="35"/>
     </row>
     <row r="125" spans="1:1" ht="15.75" customHeight="1">
-      <c r="A125" s="36"/>
+      <c r="A125" s="35"/>
     </row>
     <row r="126" spans="1:1" ht="15.75" customHeight="1">
-      <c r="A126" s="36"/>
+      <c r="A126" s="35"/>
     </row>
     <row r="127" spans="1:1" ht="15.75" customHeight="1">
-      <c r="A127" s="36"/>
+      <c r="A127" s="35"/>
     </row>
     <row r="128" spans="1:1" ht="15.75" customHeight="1">
-      <c r="A128" s="36"/>
+      <c r="A128" s="35"/>
     </row>
     <row r="129" spans="1:1" ht="15.75" customHeight="1">
-      <c r="A129" s="36"/>
+      <c r="A129" s="35"/>
     </row>
     <row r="130" spans="1:1" ht="15.75" customHeight="1">
-      <c r="A130" s="36"/>
+      <c r="A130" s="35"/>
     </row>
     <row r="131" spans="1:1" ht="15.75" customHeight="1">
-      <c r="A131" s="36"/>
+      <c r="A131" s="35"/>
     </row>
     <row r="132" spans="1:1" ht="15.75" customHeight="1">
-      <c r="A132" s="36"/>
+      <c r="A132" s="35"/>
     </row>
     <row r="133" spans="1:1" ht="15.75" customHeight="1">
-      <c r="A133" s="36"/>
+      <c r="A133" s="35"/>
     </row>
     <row r="134" spans="1:1" ht="15.75" customHeight="1">
-      <c r="A134" s="36"/>
+      <c r="A134" s="35"/>
     </row>
     <row r="135" spans="1:1" ht="15.75" customHeight="1">
-      <c r="A135" s="36"/>
+      <c r="A135" s="35"/>
     </row>
     <row r="136" spans="1:1" ht="15.75" customHeight="1">
-      <c r="A136" s="36"/>
+      <c r="A136" s="35"/>
     </row>
     <row r="137" spans="1:1" ht="15.75" customHeight="1">
-      <c r="A137" s="36"/>
+      <c r="A137" s="35"/>
     </row>
     <row r="138" spans="1:1" ht="15.75" customHeight="1">
-      <c r="A138" s="36"/>
+      <c r="A138" s="35"/>
     </row>
     <row r="139" spans="1:1" ht="15.75" customHeight="1">
-      <c r="A139" s="36"/>
+      <c r="A139" s="35"/>
     </row>
     <row r="140" spans="1:1" ht="15.75" customHeight="1">
-      <c r="A140" s="36"/>
+      <c r="A140" s="35"/>
     </row>
     <row r="141" spans="1:1" ht="15.75" customHeight="1">
-      <c r="A141" s="36"/>
+      <c r="A141" s="35"/>
     </row>
     <row r="142" spans="1:1" ht="15.75" customHeight="1">
-      <c r="A142" s="36"/>
+      <c r="A142" s="35"/>
     </row>
     <row r="143" spans="1:1" ht="15.75" customHeight="1">
-      <c r="A143" s="36"/>
+      <c r="A143" s="35"/>
     </row>
     <row r="144" spans="1:1" ht="15.75" customHeight="1">
-      <c r="A144" s="36"/>
+      <c r="A144" s="35"/>
     </row>
     <row r="145" spans="1:1" ht="15.75" customHeight="1">
-      <c r="A145" s="36"/>
+      <c r="A145" s="35"/>
     </row>
     <row r="146" spans="1:1" ht="15.75" customHeight="1">
-      <c r="A146" s="36"/>
+      <c r="A146" s="35"/>
     </row>
     <row r="147" spans="1:1" ht="15.75" customHeight="1">
-      <c r="A147" s="36"/>
+      <c r="A147" s="35"/>
     </row>
     <row r="148" spans="1:1" ht="15.75" customHeight="1">
-      <c r="A148" s="36"/>
+      <c r="A148" s="35"/>
     </row>
     <row r="149" spans="1:1" ht="15.75" customHeight="1">
-      <c r="A149" s="36"/>
+      <c r="A149" s="35"/>
     </row>
     <row r="150" spans="1:1" ht="15.75" customHeight="1">
-      <c r="A150" s="36"/>
+      <c r="A150" s="35"/>
     </row>
     <row r="151" spans="1:1" ht="15.75" customHeight="1">
-      <c r="A151" s="36"/>
+      <c r="A151" s="35"/>
     </row>
     <row r="152" spans="1:1" ht="15.75" customHeight="1">
-      <c r="A152" s="36"/>
+      <c r="A152" s="35"/>
     </row>
     <row r="153" spans="1:1" ht="15.75" customHeight="1">
-      <c r="A153" s="36"/>
+      <c r="A153" s="35"/>
     </row>
     <row r="154" spans="1:1" ht="15.75" customHeight="1">
-      <c r="A154" s="36"/>
+      <c r="A154" s="35"/>
     </row>
     <row r="155" spans="1:1" ht="15.75" customHeight="1">
-      <c r="A155" s="36"/>
+      <c r="A155" s="35"/>
     </row>
     <row r="156" spans="1:1" ht="15.75" customHeight="1">
-      <c r="A156" s="36"/>
+      <c r="A156" s="35"/>
     </row>
     <row r="157" spans="1:1" ht="15.75" customHeight="1">
-      <c r="A157" s="36"/>
+      <c r="A157" s="35"/>
     </row>
     <row r="158" spans="1:1" ht="15.75" customHeight="1">
-      <c r="A158" s="36"/>
+      <c r="A158" s="35"/>
     </row>
     <row r="159" spans="1:1" ht="15.75" customHeight="1">
-      <c r="A159" s="36"/>
+      <c r="A159" s="35"/>
     </row>
     <row r="160" spans="1:1" ht="15.75" customHeight="1">
-      <c r="A160" s="36"/>
+      <c r="A160" s="35"/>
     </row>
     <row r="161" spans="1:1" ht="15.75" customHeight="1">
-      <c r="A161" s="36"/>
+      <c r="A161" s="35"/>
     </row>
     <row r="162" spans="1:1" ht="15.75" customHeight="1">
-      <c r="A162" s="36"/>
+      <c r="A162" s="35"/>
     </row>
     <row r="163" spans="1:1" ht="15.75" customHeight="1">
-      <c r="A163" s="36"/>
+      <c r="A163" s="35"/>
     </row>
     <row r="164" spans="1:1" ht="15.75" customHeight="1">
-      <c r="A164" s="36"/>
+      <c r="A164" s="35"/>
     </row>
     <row r="165" spans="1:1" ht="15.75" customHeight="1">
-      <c r="A165" s="36"/>
+      <c r="A165" s="35"/>
     </row>
     <row r="166" spans="1:1" ht="15.75" customHeight="1">
-      <c r="A166" s="36"/>
+      <c r="A166" s="35"/>
     </row>
     <row r="167" spans="1:1" ht="15.75" customHeight="1">
-      <c r="A167" s="36"/>
+      <c r="A167" s="35"/>
     </row>
     <row r="168" spans="1:1" ht="15.75" customHeight="1">
-      <c r="A168" s="36"/>
+      <c r="A168" s="35"/>
     </row>
     <row r="169" spans="1:1" ht="15.75" customHeight="1">
-      <c r="A169" s="36"/>
+      <c r="A169" s="35"/>
     </row>
     <row r="170" spans="1:1" ht="15.75" customHeight="1">
-      <c r="A170" s="36"/>
+      <c r="A170" s="35"/>
     </row>
     <row r="171" spans="1:1" ht="15.75" customHeight="1">
-      <c r="A171" s="36"/>
+      <c r="A171" s="35"/>
     </row>
     <row r="172" spans="1:1" ht="15.75" customHeight="1">
-      <c r="A172" s="36"/>
+      <c r="A172" s="35"/>
     </row>
     <row r="173" spans="1:1" ht="15.75" customHeight="1">
-      <c r="A173" s="36"/>
+      <c r="A173" s="35"/>
     </row>
     <row r="174" spans="1:1" ht="15.75" customHeight="1">
-      <c r="A174" s="36"/>
+      <c r="A174" s="35"/>
     </row>
     <row r="175" spans="1:1" ht="15.75" customHeight="1">
-      <c r="A175" s="36"/>
+      <c r="A175" s="35"/>
     </row>
     <row r="176" spans="1:1" ht="15.75" customHeight="1">
-      <c r="A176" s="36"/>
+      <c r="A176" s="35"/>
     </row>
     <row r="177" spans="1:1" ht="15.75" customHeight="1">
-      <c r="A177" s="36"/>
+      <c r="A177" s="35"/>
     </row>
     <row r="178" spans="1:1" ht="15.75" customHeight="1">
-      <c r="A178" s="36"/>
+      <c r="A178" s="35"/>
     </row>
     <row r="179" spans="1:1" ht="15.75" customHeight="1">
-      <c r="A179" s="36"/>
+      <c r="A179" s="35"/>
     </row>
     <row r="180" spans="1:1" ht="15.75" customHeight="1">
-      <c r="A180" s="36"/>
+      <c r="A180" s="35"/>
     </row>
     <row r="181" spans="1:1" ht="15.75" customHeight="1">
-      <c r="A181" s="36"/>
+      <c r="A181" s="35"/>
     </row>
     <row r="182" spans="1:1" ht="15.75" customHeight="1">
-      <c r="A182" s="36"/>
+      <c r="A182" s="35"/>
     </row>
     <row r="183" spans="1:1" ht="15.75" customHeight="1">
-      <c r="A183" s="36"/>
+      <c r="A183" s="35"/>
     </row>
     <row r="184" spans="1:1" ht="15.75" customHeight="1">
-      <c r="A184" s="36"/>
+      <c r="A184" s="35"/>
     </row>
     <row r="185" spans="1:1" ht="15.75" customHeight="1">
-      <c r="A185" s="36"/>
+      <c r="A185" s="35"/>
     </row>
     <row r="186" spans="1:1" ht="15.75" customHeight="1">
-      <c r="A186" s="36"/>
+      <c r="A186" s="35"/>
     </row>
     <row r="187" spans="1:1" ht="15.75" customHeight="1">
-      <c r="A187" s="36"/>
+      <c r="A187" s="35"/>
     </row>
     <row r="188" spans="1:1" ht="15.75" customHeight="1">
-      <c r="A188" s="36"/>
+      <c r="A188" s="35"/>
     </row>
     <row r="189" spans="1:1" ht="15.75" customHeight="1">
-      <c r="A189" s="36"/>
+      <c r="A189" s="35"/>
     </row>
     <row r="190" spans="1:1" ht="15.75" customHeight="1">
-      <c r="A190" s="36"/>
+      <c r="A190" s="35"/>
     </row>
     <row r="191" spans="1:1" ht="15.75" customHeight="1">
-      <c r="A191" s="36"/>
+      <c r="A191" s="35"/>
     </row>
     <row r="192" spans="1:1" ht="15.75" customHeight="1">
-      <c r="A192" s="36"/>
+      <c r="A192" s="35"/>
     </row>
     <row r="193" spans="1:1" ht="15.75" customHeight="1">
-      <c r="A193" s="36"/>
+      <c r="A193" s="35"/>
     </row>
     <row r="194" spans="1:1" ht="15.75" customHeight="1">
-      <c r="A194" s="36"/>
+      <c r="A194" s="35"/>
     </row>
     <row r="195" spans="1:1" ht="15.75" customHeight="1">
-      <c r="A195" s="36"/>
+      <c r="A195" s="35"/>
     </row>
     <row r="196" spans="1:1" ht="15.75" customHeight="1">
-      <c r="A196" s="36"/>
+      <c r="A196" s="35"/>
     </row>
     <row r="197" spans="1:1" ht="15.75" customHeight="1">
-      <c r="A197" s="36"/>
+      <c r="A197" s="35"/>
     </row>
     <row r="198" spans="1:1" ht="15.75" customHeight="1">
-      <c r="A198" s="36"/>
+      <c r="A198" s="35"/>
     </row>
     <row r="199" spans="1:1" ht="15.75" customHeight="1">
-      <c r="A199" s="36"/>
+      <c r="A199" s="35"/>
     </row>
     <row r="200" spans="1:1" ht="15.75" customHeight="1">
-      <c r="A200" s="36"/>
+      <c r="A200" s="35"/>
     </row>
     <row r="201" spans="1:1" ht="15.75" customHeight="1">
-      <c r="A201" s="36"/>
+      <c r="A201" s="35"/>
     </row>
     <row r="202" spans="1:1" ht="15.75" customHeight="1">
-      <c r="A202" s="36"/>
+      <c r="A202" s="35"/>
     </row>
     <row r="203" spans="1:1" ht="15.75" customHeight="1">
-      <c r="A203" s="36"/>
+      <c r="A203" s="35"/>
     </row>
     <row r="204" spans="1:1" ht="15.75" customHeight="1">
-      <c r="A204" s="36"/>
+      <c r="A204" s="35"/>
     </row>
     <row r="205" spans="1:1" ht="15.75" customHeight="1">
-      <c r="A205" s="36"/>
+      <c r="A205" s="35"/>
     </row>
     <row r="206" spans="1:1" ht="15.75" customHeight="1">
-      <c r="A206" s="36"/>
+      <c r="A206" s="35"/>
     </row>
     <row r="207" spans="1:1" ht="15.75" customHeight="1">
-      <c r="A207" s="36"/>
+      <c r="A207" s="35"/>
     </row>
     <row r="208" spans="1:1" ht="15.75" customHeight="1">
-      <c r="A208" s="36"/>
+      <c r="A208" s="35"/>
     </row>
     <row r="209" spans="1:1" ht="15.75" customHeight="1">
-      <c r="A209" s="36"/>
+      <c r="A209" s="35"/>
     </row>
     <row r="210" spans="1:1" ht="15.75" customHeight="1">
-      <c r="A210" s="36"/>
+      <c r="A210" s="35"/>
     </row>
     <row r="211" spans="1:1" ht="15.75" customHeight="1">
-      <c r="A211" s="36"/>
+      <c r="A211" s="35"/>
     </row>
     <row r="212" spans="1:1" ht="15.75" customHeight="1">
-      <c r="A212" s="36"/>
+      <c r="A212" s="35"/>
     </row>
     <row r="213" spans="1:1" ht="15.75" customHeight="1">
-      <c r="A213" s="36"/>
+      <c r="A213" s="35"/>
     </row>
     <row r="214" spans="1:1" ht="15.75" customHeight="1">
-      <c r="A214" s="36"/>
+      <c r="A214" s="35"/>
     </row>
     <row r="215" spans="1:1" ht="15.75" customHeight="1">
-      <c r="A215" s="36"/>
+      <c r="A215" s="35"/>
     </row>
     <row r="216" spans="1:1" ht="15.75" customHeight="1">
-      <c r="A216" s="36"/>
+      <c r="A216" s="35"/>
     </row>
     <row r="217" spans="1:1" ht="15.75" customHeight="1">
-      <c r="A217" s="36"/>
+      <c r="A217" s="35"/>
     </row>
     <row r="218" spans="1:1" ht="15.75" customHeight="1">
-      <c r="A218" s="36"/>
+      <c r="A218" s="35"/>
     </row>
     <row r="219" spans="1:1" ht="15.75" customHeight="1">
-      <c r="A219" s="36"/>
+      <c r="A219" s="35"/>
     </row>
     <row r="220" spans="1:1" ht="15.75" customHeight="1">
-      <c r="A220" s="36"/>
+      <c r="A220" s="35"/>
     </row>
     <row r="221" spans="1:1" ht="15.75" customHeight="1">
-      <c r="A221" s="36"/>
+      <c r="A221" s="35"/>
     </row>
     <row r="222" spans="1:1" ht="15.75" customHeight="1">
-      <c r="A222" s="36"/>
+      <c r="A222" s="35"/>
     </row>
     <row r="223" spans="1:1" ht="15.75" customHeight="1">
-      <c r="A223" s="36"/>
+      <c r="A223" s="35"/>
     </row>
     <row r="224" spans="1:1" ht="15.75" customHeight="1">
-      <c r="A224" s="36"/>
+      <c r="A224" s="35"/>
     </row>
     <row r="225" spans="1:1" ht="15.75" customHeight="1">
-      <c r="A225" s="36"/>
+      <c r="A225" s="35"/>
     </row>
     <row r="226" spans="1:1" ht="15.75" customHeight="1">
-      <c r="A226" s="36"/>
+      <c r="A226" s="35"/>
     </row>
     <row r="227" spans="1:1" ht="15.75" customHeight="1">
-      <c r="A227" s="36"/>
+      <c r="A227" s="35"/>
     </row>
     <row r="228" spans="1:1" ht="15.75" customHeight="1">
-      <c r="A228" s="36"/>
+      <c r="A228" s="35"/>
     </row>
     <row r="229" spans="1:1" ht="15.75" customHeight="1">
-      <c r="A229" s="36"/>
+      <c r="A229" s="35"/>
     </row>
     <row r="230" spans="1:1" ht="15.75" customHeight="1">
-      <c r="A230" s="36"/>
+      <c r="A230" s="35"/>
     </row>
     <row r="231" spans="1:1" ht="15.75" customHeight="1">
-      <c r="A231" s="36"/>
+      <c r="A231" s="35"/>
     </row>
     <row r="232" spans="1:1" ht="15.75" customHeight="1">
-      <c r="A232" s="36"/>
+      <c r="A232" s="35"/>
     </row>
     <row r="233" spans="1:1" ht="15.75" customHeight="1">
-      <c r="A233" s="36"/>
+      <c r="A233" s="35"/>
     </row>
     <row r="234" spans="1:1" ht="15.75" customHeight="1">
-      <c r="A234" s="36"/>
+      <c r="A234" s="35"/>
     </row>
     <row r="235" spans="1:1" ht="15.75" customHeight="1">
-      <c r="A235" s="36"/>
+      <c r="A235" s="35"/>
     </row>
     <row r="236" spans="1:1" ht="15.75" customHeight="1">
-      <c r="A236" s="36"/>
+      <c r="A236" s="35"/>
     </row>
     <row r="237" spans="1:1" ht="15.75" customHeight="1">
-      <c r="A237" s="36"/>
+      <c r="A237" s="35"/>
     </row>
     <row r="238" spans="1:1" ht="15.75" customHeight="1">
-      <c r="A238" s="36"/>
+      <c r="A238" s="35"/>
     </row>
     <row r="239" spans="1:1" ht="15.75" customHeight="1">
-      <c r="A239" s="36"/>
+      <c r="A239" s="35"/>
     </row>
     <row r="240" spans="1:1" ht="15.75" customHeight="1">
-      <c r="A240" s="36"/>
+      <c r="A240" s="35"/>
     </row>
     <row r="241" spans="1:1" ht="15.75" customHeight="1">
-      <c r="A241" s="36"/>
+      <c r="A241" s="35"/>
     </row>
     <row r="242" spans="1:1" ht="15.75" customHeight="1">
-      <c r="A242" s="36"/>
+      <c r="A242" s="35"/>
     </row>
     <row r="243" spans="1:1" ht="15.75" customHeight="1">
-      <c r="A243" s="36"/>
+      <c r="A243" s="35"/>
     </row>
     <row r="244" spans="1:1" ht="15.75" customHeight="1">
-      <c r="A244" s="36"/>
+      <c r="A244" s="35"/>
     </row>
     <row r="245" spans="1:1" ht="15.75" customHeight="1">
-      <c r="A245" s="36"/>
+      <c r="A245" s="35"/>
     </row>
     <row r="246" spans="1:1" ht="15.75" customHeight="1">
-      <c r="A246" s="36"/>
+      <c r="A246" s="35"/>
     </row>
     <row r="247" spans="1:1" ht="15.75" customHeight="1">
-      <c r="A247" s="36"/>
+      <c r="A247" s="35"/>
     </row>
     <row r="248" spans="1:1" ht="15.75" customHeight="1">
-      <c r="A248" s="36"/>
+      <c r="A248" s="35"/>
     </row>
     <row r="249" spans="1:1" ht="15.75" customHeight="1">
-      <c r="A249" s="36"/>
+      <c r="A249" s="35"/>
     </row>
     <row r="250" spans="1:1" ht="15.75" customHeight="1">
-      <c r="A250" s="36"/>
+      <c r="A250" s="35"/>
     </row>
     <row r="251" spans="1:1" ht="15.75" customHeight="1">
-      <c r="A251" s="36"/>
+      <c r="A251" s="35"/>
     </row>
     <row r="252" spans="1:1" ht="15.75" customHeight="1">
-      <c r="A252" s="36"/>
+      <c r="A252" s="35"/>
     </row>
     <row r="253" spans="1:1" ht="15.75" customHeight="1">
-      <c r="A253" s="36"/>
+      <c r="A253" s="35"/>
     </row>
     <row r="254" spans="1:1" ht="15.75" customHeight="1">
-      <c r="A254" s="36"/>
+      <c r="A254" s="35"/>
     </row>
     <row r="255" spans="1:1" ht="15.75" customHeight="1">
-      <c r="A255" s="36"/>
+      <c r="A255" s="35"/>
     </row>
     <row r="256" spans="1:1" ht="15.75" customHeight="1">
-      <c r="A256" s="36"/>
+      <c r="A256" s="35"/>
     </row>
     <row r="257" spans="1:1" ht="15.75" customHeight="1">
-      <c r="A257" s="36"/>
+      <c r="A257" s="35"/>
     </row>
     <row r="258" spans="1:1" ht="15.75" customHeight="1">
-      <c r="A258" s="36"/>
+      <c r="A258" s="35"/>
     </row>
     <row r="259" spans="1:1" ht="15.75" customHeight="1">
-      <c r="A259" s="36"/>
+      <c r="A259" s="35"/>
     </row>
     <row r="260" spans="1:1" ht="15.75" customHeight="1">
-      <c r="A260" s="36"/>
+      <c r="A260" s="35"/>
     </row>
     <row r="261" spans="1:1" ht="15.75" customHeight="1">
-      <c r="A261" s="36"/>
+      <c r="A261" s="35"/>
     </row>
     <row r="262" spans="1:1" ht="15.75" customHeight="1">
-      <c r="A262" s="36"/>
+      <c r="A262" s="35"/>
     </row>
     <row r="263" spans="1:1" ht="15.75" customHeight="1">
-      <c r="A263" s="36"/>
+      <c r="A263" s="35"/>
     </row>
     <row r="264" spans="1:1" ht="15.75" customHeight="1">
-      <c r="A264" s="36"/>
+      <c r="A264" s="35"/>
     </row>
     <row r="265" spans="1:1" ht="15.75" customHeight="1">
-      <c r="A265" s="36"/>
+      <c r="A265" s="35"/>
     </row>
     <row r="266" spans="1:1" ht="15.75" customHeight="1">
-      <c r="A266" s="36"/>
+      <c r="A266" s="35"/>
     </row>
     <row r="267" spans="1:1" ht="15.75" customHeight="1">
-      <c r="A267" s="36"/>
+      <c r="A267" s="35"/>
     </row>
     <row r="268" spans="1:1" ht="15.75" customHeight="1"/>
     <row r="269" spans="1:1" ht="15.75" customHeight="1"/>
@@ -5634,7 +5634,7 @@
   </sheetData>
   <autoFilter ref="A1:H76"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0" footer="0"/>
-  <pageSetup paperSize="9" orientation="portrait"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
       <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="18">
@@ -5785,670 +5785,670 @@
   </cols>
   <sheetData>
     <row r="2" spans="1:26">
-      <c r="A2" s="53" t="s">
+      <c r="A2" s="52" t="s">
         <v>174</v>
       </c>
-      <c r="B2" s="53" t="s">
+      <c r="B2" s="52" t="s">
         <v>174</v>
       </c>
-      <c r="C2" s="53" t="s">
+      <c r="C2" s="52" t="s">
         <v>174</v>
       </c>
-      <c r="D2" s="53" t="s">
+      <c r="D2" s="52" t="s">
         <v>174</v>
       </c>
-      <c r="E2" s="53" t="s">
+      <c r="E2" s="52" t="s">
         <v>174</v>
       </c>
-      <c r="F2" s="53" t="s">
+      <c r="F2" s="52" t="s">
         <v>174</v>
       </c>
-      <c r="G2" s="53" t="s">
+      <c r="G2" s="52" t="s">
         <v>174</v>
       </c>
-      <c r="H2" s="53" t="s">
+      <c r="H2" s="52" t="s">
         <v>174</v>
       </c>
-      <c r="I2" s="53" t="s">
+      <c r="I2" s="52" t="s">
         <v>174</v>
       </c>
-      <c r="J2" s="53" t="s">
+      <c r="J2" s="52" t="s">
         <v>174</v>
       </c>
-      <c r="K2" s="53" t="s">
+      <c r="K2" s="52" t="s">
         <v>174</v>
       </c>
-      <c r="L2" s="53" t="s">
+      <c r="L2" s="52" t="s">
         <v>174</v>
       </c>
-      <c r="M2" s="53" t="s">
+      <c r="M2" s="52" t="s">
         <v>174</v>
       </c>
-      <c r="N2" s="53" t="s">
+      <c r="N2" s="52" t="s">
         <v>174</v>
       </c>
-      <c r="R2" s="53" t="s">
+      <c r="R2" s="52" t="s">
         <v>174</v>
       </c>
-      <c r="S2" s="53" t="s">
+      <c r="S2" s="52" t="s">
         <v>174</v>
       </c>
-      <c r="T2" s="53" t="s">
+      <c r="T2" s="52" t="s">
         <v>174</v>
       </c>
-      <c r="U2" s="53" t="s">
+      <c r="U2" s="52" t="s">
         <v>174</v>
       </c>
-      <c r="V2" s="53" t="s">
+      <c r="V2" s="52" t="s">
         <v>175</v>
       </c>
-      <c r="W2" s="53" t="s">
+      <c r="W2" s="52" t="s">
         <v>176</v>
       </c>
-      <c r="X2" s="53"/>
-      <c r="Y2" s="53" t="s">
+      <c r="X2" s="52"/>
+      <c r="Y2" s="52" t="s">
         <v>175</v>
       </c>
-      <c r="Z2" s="53" t="s">
+      <c r="Z2" s="52" t="s">
         <v>175</v>
       </c>
     </row>
     <row r="3" spans="1:26">
-      <c r="A3" s="53" t="s">
+      <c r="A3" s="52" t="s">
         <v>177</v>
       </c>
-      <c r="B3" s="53" t="s">
+      <c r="B3" s="52" t="s">
         <v>178</v>
       </c>
-      <c r="C3" s="53" t="s">
+      <c r="C3" s="52" t="s">
         <v>179</v>
       </c>
-      <c r="D3" s="53" t="s">
+      <c r="D3" s="52" t="s">
         <v>177</v>
       </c>
-      <c r="E3" s="53" t="s">
+      <c r="E3" s="52" t="s">
         <v>177</v>
       </c>
-      <c r="F3" s="53" t="s">
+      <c r="F3" s="52" t="s">
         <v>180</v>
       </c>
-      <c r="G3" s="53" t="s">
+      <c r="G3" s="52" t="s">
         <v>181</v>
       </c>
-      <c r="H3" s="53" t="s">
+      <c r="H3" s="52" t="s">
         <v>182</v>
       </c>
-      <c r="I3" s="53" t="s">
+      <c r="I3" s="52" t="s">
         <v>183</v>
       </c>
-      <c r="J3" s="53" t="s">
+      <c r="J3" s="52" t="s">
         <v>184</v>
       </c>
-      <c r="K3" s="53" t="s">
+      <c r="K3" s="52" t="s">
         <v>185</v>
       </c>
-      <c r="L3" s="53" t="s">
+      <c r="L3" s="52" t="s">
         <v>181</v>
       </c>
-      <c r="M3" s="53" t="s">
+      <c r="M3" s="52" t="s">
         <v>181</v>
       </c>
-      <c r="N3" s="53" t="s">
+      <c r="N3" s="52" t="s">
         <v>186</v>
       </c>
-      <c r="R3" s="53" t="s">
+      <c r="R3" s="52" t="s">
         <v>187</v>
       </c>
-      <c r="S3" s="53" t="s">
+      <c r="S3" s="52" t="s">
         <v>188</v>
       </c>
-      <c r="T3" s="53" t="s">
+      <c r="T3" s="52" t="s">
         <v>189</v>
       </c>
-      <c r="U3" s="53" t="s">
+      <c r="U3" s="52" t="s">
         <v>190</v>
       </c>
-      <c r="V3" s="53" t="s">
+      <c r="V3" s="52" t="s">
         <v>191</v>
       </c>
-      <c r="W3" s="53" t="s">
+      <c r="W3" s="52" t="s">
         <v>178</v>
       </c>
-      <c r="X3" s="53"/>
-      <c r="Y3" s="53" t="s">
+      <c r="X3" s="52"/>
+      <c r="Y3" s="52" t="s">
         <v>192</v>
       </c>
-      <c r="Z3" s="53" t="s">
+      <c r="Z3" s="52" t="s">
         <v>177</v>
       </c>
     </row>
     <row r="4" spans="1:26">
-      <c r="A4" s="53" t="s">
+      <c r="A4" s="52" t="s">
         <v>193</v>
       </c>
-      <c r="B4" s="53" t="s">
+      <c r="B4" s="52" t="s">
         <v>183</v>
       </c>
-      <c r="C4" s="53" t="s">
+      <c r="C4" s="52" t="s">
         <v>194</v>
       </c>
-      <c r="D4" s="53" t="s">
+      <c r="D4" s="52" t="s">
         <v>195</v>
       </c>
-      <c r="E4" s="53" t="s">
+      <c r="E4" s="52" t="s">
         <v>196</v>
       </c>
-      <c r="F4" s="53" t="s">
+      <c r="F4" s="52" t="s">
         <v>183</v>
       </c>
-      <c r="G4" s="53" t="s">
+      <c r="G4" s="52" t="s">
         <v>197</v>
       </c>
-      <c r="H4" s="53" t="s">
+      <c r="H4" s="52" t="s">
         <v>198</v>
       </c>
-      <c r="I4" s="54" t="s">
+      <c r="I4" s="53" t="s">
         <v>188</v>
       </c>
-      <c r="J4" s="36" t="s">
+      <c r="J4" s="35" t="s">
         <v>199</v>
       </c>
-      <c r="K4" s="53" t="s">
+      <c r="K4" s="52" t="s">
         <v>193</v>
       </c>
-      <c r="L4" s="53" t="s">
+      <c r="L4" s="52" t="s">
         <v>197</v>
       </c>
-      <c r="M4" s="53" t="s">
+      <c r="M4" s="52" t="s">
         <v>200</v>
       </c>
-      <c r="N4" s="53" t="s">
+      <c r="N4" s="52" t="s">
         <v>189</v>
       </c>
-      <c r="R4" s="53" t="s">
+      <c r="R4" s="52" t="s">
         <v>201</v>
       </c>
-      <c r="S4" s="53" t="s">
+      <c r="S4" s="52" t="s">
         <v>178</v>
       </c>
-      <c r="T4" s="53" t="s">
+      <c r="T4" s="52" t="s">
         <v>202</v>
       </c>
-      <c r="U4" s="53" t="s">
+      <c r="U4" s="52" t="s">
         <v>203</v>
       </c>
-      <c r="V4" s="53" t="s">
+      <c r="V4" s="52" t="s">
         <v>204</v>
       </c>
-      <c r="W4" s="53" t="s">
+      <c r="W4" s="52" t="s">
         <v>205</v>
       </c>
-      <c r="X4" s="53"/>
-      <c r="Y4" s="53" t="s">
+      <c r="X4" s="52"/>
+      <c r="Y4" s="52" t="s">
         <v>206</v>
       </c>
-      <c r="Z4" s="53" t="s">
+      <c r="Z4" s="52" t="s">
         <v>178</v>
       </c>
     </row>
     <row r="5" spans="1:26">
-      <c r="A5" s="53"/>
-      <c r="B5" s="53" t="s">
+      <c r="A5" s="52"/>
+      <c r="B5" s="52" t="s">
         <v>193</v>
       </c>
-      <c r="C5" s="53" t="s">
+      <c r="C5" s="52" t="s">
         <v>207</v>
       </c>
-      <c r="D5" s="53" t="s">
+      <c r="D5" s="52" t="s">
         <v>193</v>
       </c>
-      <c r="E5" s="53" t="s">
+      <c r="E5" s="52" t="s">
         <v>208</v>
       </c>
-      <c r="F5" s="53" t="s">
+      <c r="F5" s="52" t="s">
         <v>193</v>
       </c>
-      <c r="G5" s="53" t="s">
+      <c r="G5" s="52" t="s">
         <v>193</v>
       </c>
-      <c r="H5" s="53" t="s">
+      <c r="H5" s="52" t="s">
         <v>209</v>
       </c>
-      <c r="I5" s="54" t="s">
+      <c r="I5" s="53" t="s">
         <v>186</v>
       </c>
-      <c r="J5" s="53" t="s">
+      <c r="J5" s="52" t="s">
         <v>209</v>
       </c>
-      <c r="L5" s="54" t="s">
+      <c r="L5" s="53" t="s">
         <v>196</v>
       </c>
-      <c r="M5" s="53" t="s">
+      <c r="M5" s="52" t="s">
         <v>197</v>
       </c>
-      <c r="N5" s="53" t="s">
+      <c r="N5" s="52" t="s">
         <v>197</v>
       </c>
-      <c r="R5" s="53" t="s">
+      <c r="R5" s="52" t="s">
         <v>210</v>
       </c>
-      <c r="S5" s="53" t="s">
+      <c r="S5" s="52" t="s">
         <v>211</v>
       </c>
-      <c r="T5" s="53" t="s">
+      <c r="T5" s="52" t="s">
         <v>212</v>
       </c>
-      <c r="V5" s="53" t="s">
+      <c r="V5" s="52" t="s">
         <v>213</v>
       </c>
-      <c r="X5" s="53"/>
-      <c r="Z5" s="53" t="s">
+      <c r="X5" s="52"/>
+      <c r="Z5" s="52" t="s">
         <v>214</v>
       </c>
     </row>
     <row r="6" spans="1:26">
-      <c r="A6" s="53"/>
-      <c r="B6" s="53"/>
-      <c r="C6" s="53" t="s">
+      <c r="A6" s="52"/>
+      <c r="B6" s="52"/>
+      <c r="C6" s="52" t="s">
         <v>193</v>
       </c>
-      <c r="D6" s="53"/>
-      <c r="E6" s="53" t="s">
+      <c r="D6" s="52"/>
+      <c r="E6" s="52" t="s">
         <v>193</v>
       </c>
-      <c r="F6" s="53"/>
-      <c r="G6" s="53"/>
-      <c r="I6" s="53" t="s">
+      <c r="F6" s="52"/>
+      <c r="G6" s="52"/>
+      <c r="I6" s="52" t="s">
         <v>209</v>
       </c>
-      <c r="L6" s="54" t="s">
+      <c r="L6" s="53" t="s">
         <v>208</v>
       </c>
-      <c r="M6" s="54" t="s">
+      <c r="M6" s="53" t="s">
         <v>196</v>
       </c>
-      <c r="N6" s="54" t="s">
+      <c r="N6" s="53" t="s">
         <v>196</v>
       </c>
-      <c r="R6" s="53" t="s">
+      <c r="R6" s="52" t="s">
         <v>193</v>
       </c>
-      <c r="S6" s="53" t="s">
+      <c r="S6" s="52" t="s">
         <v>193</v>
       </c>
-      <c r="T6" s="53" t="s">
+      <c r="T6" s="52" t="s">
         <v>196</v>
       </c>
-      <c r="V6" s="53" t="s">
+      <c r="V6" s="52" t="s">
         <v>205</v>
       </c>
     </row>
     <row r="7" spans="1:26">
-      <c r="A7" s="53"/>
-      <c r="B7" s="53"/>
-      <c r="C7" s="53"/>
-      <c r="D7" s="53"/>
-      <c r="E7" s="53"/>
-      <c r="F7" s="53"/>
-      <c r="G7" s="53"/>
-      <c r="L7" s="53" t="s">
+      <c r="A7" s="52"/>
+      <c r="B7" s="52"/>
+      <c r="C7" s="52"/>
+      <c r="D7" s="52"/>
+      <c r="E7" s="52"/>
+      <c r="F7" s="52"/>
+      <c r="G7" s="52"/>
+      <c r="L7" s="52" t="s">
         <v>193</v>
       </c>
-      <c r="M7" s="54" t="s">
+      <c r="M7" s="53" t="s">
         <v>208</v>
       </c>
-      <c r="N7" s="53" t="s">
+      <c r="N7" s="52" t="s">
         <v>215</v>
       </c>
-      <c r="T7" s="53" t="s">
+      <c r="T7" s="52" t="s">
         <v>193</v>
       </c>
     </row>
     <row r="8" spans="1:26" ht="15" customHeight="1">
-      <c r="A8" s="53"/>
-      <c r="B8" s="53"/>
-      <c r="C8" s="53"/>
-      <c r="D8" s="53"/>
-      <c r="E8" s="53"/>
-      <c r="F8" s="53"/>
-      <c r="G8" s="53"/>
-      <c r="M8" s="53" t="s">
+      <c r="A8" s="52"/>
+      <c r="B8" s="52"/>
+      <c r="C8" s="52"/>
+      <c r="D8" s="52"/>
+      <c r="E8" s="52"/>
+      <c r="F8" s="52"/>
+      <c r="G8" s="52"/>
+      <c r="M8" s="52" t="s">
         <v>193</v>
       </c>
-      <c r="N8" s="54" t="s">
+      <c r="N8" s="53" t="s">
         <v>208</v>
       </c>
     </row>
     <row r="9" spans="1:26" ht="15" customHeight="1">
-      <c r="A9" s="53"/>
-      <c r="B9" s="53"/>
-      <c r="C9" s="53"/>
-      <c r="D9" s="53"/>
-      <c r="E9" s="53"/>
-      <c r="F9" s="53"/>
-      <c r="G9" s="53"/>
-      <c r="N9" s="53" t="s">
+      <c r="A9" s="52"/>
+      <c r="B9" s="52"/>
+      <c r="C9" s="52"/>
+      <c r="D9" s="52"/>
+      <c r="E9" s="52"/>
+      <c r="F9" s="52"/>
+      <c r="G9" s="52"/>
+      <c r="N9" s="52" t="s">
         <v>193</v>
       </c>
     </row>
     <row r="10" spans="1:26" ht="15" customHeight="1">
-      <c r="A10" s="53"/>
-      <c r="B10" s="53"/>
-      <c r="C10" s="53"/>
-      <c r="D10" s="53"/>
-      <c r="E10" s="53"/>
-      <c r="F10" s="53"/>
-      <c r="G10" s="53"/>
+      <c r="A10" s="52"/>
+      <c r="B10" s="52"/>
+      <c r="C10" s="52"/>
+      <c r="D10" s="52"/>
+      <c r="E10" s="52"/>
+      <c r="F10" s="52"/>
+      <c r="G10" s="52"/>
     </row>
     <row r="11" spans="1:26" ht="15" customHeight="1">
-      <c r="A11" s="53"/>
-      <c r="B11" s="53"/>
-      <c r="C11" s="53"/>
-      <c r="D11" s="53"/>
-      <c r="E11" s="53"/>
-      <c r="F11" s="53"/>
-      <c r="G11" s="53"/>
+      <c r="A11" s="52"/>
+      <c r="B11" s="52"/>
+      <c r="C11" s="52"/>
+      <c r="D11" s="52"/>
+      <c r="E11" s="52"/>
+      <c r="F11" s="52"/>
+      <c r="G11" s="52"/>
     </row>
     <row r="12" spans="1:26" ht="15" customHeight="1">
-      <c r="A12" s="53" t="s">
+      <c r="A12" s="52" t="s">
         <v>174</v>
       </c>
-      <c r="B12" s="53" t="s">
+      <c r="B12" s="52" t="s">
         <v>174</v>
       </c>
-      <c r="C12" s="53"/>
-      <c r="D12" s="53"/>
-      <c r="E12" s="53"/>
-      <c r="F12" s="53"/>
-      <c r="G12" s="53"/>
+      <c r="C12" s="52"/>
+      <c r="D12" s="52"/>
+      <c r="E12" s="52"/>
+      <c r="F12" s="52"/>
+      <c r="G12" s="52"/>
     </row>
     <row r="13" spans="1:26" ht="15" customHeight="1">
-      <c r="A13" s="53" t="s">
+      <c r="A13" s="52" t="s">
         <v>203</v>
       </c>
-      <c r="B13" s="53" t="s">
+      <c r="B13" s="52" t="s">
         <v>177</v>
       </c>
-      <c r="C13" s="53"/>
-      <c r="D13" s="53"/>
-      <c r="E13" s="53"/>
-      <c r="F13" s="53"/>
-      <c r="G13" s="53"/>
+      <c r="C13" s="52"/>
+      <c r="D13" s="52"/>
+      <c r="E13" s="52"/>
+      <c r="F13" s="52"/>
+      <c r="G13" s="52"/>
     </row>
     <row r="14" spans="1:26" ht="15" customHeight="1">
-      <c r="A14" s="53" t="s">
+      <c r="A14" s="52" t="s">
         <v>216</v>
       </c>
-      <c r="B14" s="53" t="s">
+      <c r="B14" s="52" t="s">
         <v>178</v>
       </c>
-      <c r="C14" s="53"/>
-      <c r="D14" s="53"/>
-      <c r="E14" s="53"/>
-      <c r="F14" s="53"/>
-      <c r="G14" s="53"/>
+      <c r="C14" s="52"/>
+      <c r="D14" s="52"/>
+      <c r="E14" s="52"/>
+      <c r="F14" s="52"/>
+      <c r="G14" s="52"/>
     </row>
     <row r="15" spans="1:26" ht="15" customHeight="1">
-      <c r="A15" s="53" t="s">
+      <c r="A15" s="52" t="s">
         <v>217</v>
       </c>
-      <c r="B15" s="53" t="s">
+      <c r="B15" s="52" t="s">
         <v>218</v>
       </c>
-      <c r="C15" s="53"/>
-      <c r="D15" s="53"/>
-      <c r="E15" s="53"/>
-      <c r="F15" s="53"/>
-      <c r="G15" s="53"/>
+      <c r="C15" s="52"/>
+      <c r="D15" s="52"/>
+      <c r="E15" s="52"/>
+      <c r="F15" s="52"/>
+      <c r="G15" s="52"/>
     </row>
     <row r="16" spans="1:26" ht="15" customHeight="1">
-      <c r="A16" s="53"/>
-      <c r="B16" s="53" t="s">
+      <c r="A16" s="52"/>
+      <c r="B16" s="52" t="s">
         <v>193</v>
       </c>
-      <c r="C16" s="53"/>
-      <c r="D16" s="53"/>
-      <c r="E16" s="53"/>
-      <c r="F16" s="53"/>
-      <c r="G16" s="53"/>
+      <c r="C16" s="52"/>
+      <c r="D16" s="52"/>
+      <c r="E16" s="52"/>
+      <c r="F16" s="52"/>
+      <c r="G16" s="52"/>
     </row>
     <row r="17" spans="1:7" ht="15" customHeight="1">
-      <c r="A17" s="53"/>
-      <c r="B17" s="53"/>
-      <c r="C17" s="53"/>
-      <c r="D17" s="53"/>
-      <c r="E17" s="53"/>
-      <c r="F17" s="53"/>
-      <c r="G17" s="53"/>
+      <c r="A17" s="52"/>
+      <c r="B17" s="52"/>
+      <c r="C17" s="52"/>
+      <c r="D17" s="52"/>
+      <c r="E17" s="52"/>
+      <c r="F17" s="52"/>
+      <c r="G17" s="52"/>
     </row>
     <row r="18" spans="1:7" ht="15" customHeight="1">
-      <c r="A18" s="53"/>
-      <c r="B18" s="53"/>
-      <c r="C18" s="53"/>
-      <c r="D18" s="53"/>
-      <c r="E18" s="53"/>
-      <c r="F18" s="53"/>
-      <c r="G18" s="53"/>
+      <c r="A18" s="52"/>
+      <c r="B18" s="52"/>
+      <c r="C18" s="52"/>
+      <c r="D18" s="52"/>
+      <c r="E18" s="52"/>
+      <c r="F18" s="52"/>
+      <c r="G18" s="52"/>
     </row>
     <row r="19" spans="1:7" ht="15" customHeight="1">
-      <c r="A19" s="53"/>
-      <c r="B19" s="53"/>
-      <c r="C19" s="53"/>
-      <c r="D19" s="53"/>
-      <c r="E19" s="53"/>
-      <c r="F19" s="53"/>
-      <c r="G19" s="53"/>
+      <c r="A19" s="52"/>
+      <c r="B19" s="52"/>
+      <c r="C19" s="52"/>
+      <c r="D19" s="52"/>
+      <c r="E19" s="52"/>
+      <c r="F19" s="52"/>
+      <c r="G19" s="52"/>
     </row>
     <row r="20" spans="1:7" ht="15" customHeight="1">
-      <c r="A20" s="53"/>
-      <c r="B20" s="53"/>
-      <c r="C20" s="53"/>
-      <c r="D20" s="53"/>
-      <c r="E20" s="53"/>
-      <c r="F20" s="53"/>
-      <c r="G20" s="53"/>
+      <c r="A20" s="52"/>
+      <c r="B20" s="52"/>
+      <c r="C20" s="52"/>
+      <c r="D20" s="52"/>
+      <c r="E20" s="52"/>
+      <c r="F20" s="52"/>
+      <c r="G20" s="52"/>
     </row>
     <row r="21" spans="1:7" ht="15.75" customHeight="1">
-      <c r="A21" s="53" t="s">
+      <c r="A21" s="52" t="s">
         <v>174</v>
       </c>
-      <c r="B21" s="53" t="s">
+      <c r="B21" s="52" t="s">
         <v>174</v>
       </c>
-      <c r="C21" s="53" t="s">
+      <c r="C21" s="52" t="s">
         <v>174</v>
       </c>
-      <c r="D21" s="53"/>
-      <c r="E21" s="53"/>
-      <c r="F21" s="53"/>
-      <c r="G21" s="53"/>
+      <c r="D21" s="52"/>
+      <c r="E21" s="52"/>
+      <c r="F21" s="52"/>
+      <c r="G21" s="52"/>
     </row>
     <row r="22" spans="1:7" ht="15.75" customHeight="1">
-      <c r="A22" s="53" t="s">
+      <c r="A22" s="52" t="s">
         <v>177</v>
       </c>
-      <c r="B22" s="53" t="s">
+      <c r="B22" s="52" t="s">
         <v>177</v>
       </c>
-      <c r="C22" s="53" t="s">
+      <c r="C22" s="52" t="s">
         <v>219</v>
       </c>
-      <c r="D22" s="53"/>
-      <c r="E22" s="53"/>
-      <c r="F22" s="53"/>
-      <c r="G22" s="53"/>
+      <c r="D22" s="52"/>
+      <c r="E22" s="52"/>
+      <c r="F22" s="52"/>
+      <c r="G22" s="52"/>
     </row>
     <row r="23" spans="1:7" ht="15.75" customHeight="1">
-      <c r="A23" s="53" t="s">
+      <c r="A23" s="52" t="s">
         <v>178</v>
       </c>
-      <c r="B23" s="53" t="s">
+      <c r="B23" s="52" t="s">
         <v>220</v>
       </c>
-      <c r="C23" s="53" t="s">
+      <c r="C23" s="52" t="s">
         <v>221</v>
       </c>
-      <c r="D23" s="53"/>
-      <c r="E23" s="53"/>
-      <c r="F23" s="53"/>
-      <c r="G23" s="53"/>
+      <c r="D23" s="52"/>
+      <c r="E23" s="52"/>
+      <c r="F23" s="52"/>
+      <c r="G23" s="52"/>
     </row>
     <row r="24" spans="1:7" ht="15.75" customHeight="1">
-      <c r="A24" s="53" t="s">
+      <c r="A24" s="52" t="s">
         <v>222</v>
       </c>
-      <c r="B24" s="53" t="s">
+      <c r="B24" s="52" t="s">
         <v>193</v>
       </c>
-      <c r="C24" s="53" t="s">
+      <c r="C24" s="52" t="s">
         <v>193</v>
       </c>
-      <c r="D24" s="53"/>
-      <c r="E24" s="53"/>
-      <c r="F24" s="53"/>
-      <c r="G24" s="53"/>
+      <c r="D24" s="52"/>
+      <c r="E24" s="52"/>
+      <c r="F24" s="52"/>
+      <c r="G24" s="52"/>
     </row>
     <row r="25" spans="1:7" ht="15.75" customHeight="1">
-      <c r="A25" s="53" t="s">
+      <c r="A25" s="52" t="s">
         <v>193</v>
       </c>
-      <c r="B25" s="53"/>
-      <c r="C25" s="53"/>
-      <c r="D25" s="53"/>
-      <c r="E25" s="53"/>
-      <c r="F25" s="53"/>
-      <c r="G25" s="53"/>
+      <c r="B25" s="52"/>
+      <c r="C25" s="52"/>
+      <c r="D25" s="52"/>
+      <c r="E25" s="52"/>
+      <c r="F25" s="52"/>
+      <c r="G25" s="52"/>
     </row>
     <row r="26" spans="1:7" ht="15.75" customHeight="1">
-      <c r="A26" s="53"/>
-      <c r="B26" s="53"/>
-      <c r="C26" s="53"/>
-      <c r="D26" s="53"/>
-      <c r="E26" s="53"/>
-      <c r="F26" s="53"/>
-      <c r="G26" s="53"/>
+      <c r="A26" s="52"/>
+      <c r="B26" s="52"/>
+      <c r="C26" s="52"/>
+      <c r="D26" s="52"/>
+      <c r="E26" s="52"/>
+      <c r="F26" s="52"/>
+      <c r="G26" s="52"/>
     </row>
     <row r="27" spans="1:7" ht="15.75" customHeight="1">
-      <c r="A27" s="53" t="s">
+      <c r="A27" s="52" t="s">
         <v>174</v>
       </c>
-      <c r="B27" s="53" t="s">
+      <c r="B27" s="52" t="s">
         <v>174</v>
       </c>
-      <c r="C27" s="53" t="s">
+      <c r="C27" s="52" t="s">
         <v>174</v>
       </c>
-      <c r="D27" s="53"/>
-      <c r="E27" s="53"/>
-      <c r="F27" s="53"/>
-      <c r="G27" s="53"/>
+      <c r="D27" s="52"/>
+      <c r="E27" s="52"/>
+      <c r="F27" s="52"/>
+      <c r="G27" s="52"/>
     </row>
     <row r="28" spans="1:7" ht="15.75" customHeight="1">
-      <c r="A28" s="53" t="s">
+      <c r="A28" s="52" t="s">
         <v>223</v>
       </c>
-      <c r="B28" s="53" t="s">
+      <c r="B28" s="52" t="s">
         <v>177</v>
       </c>
-      <c r="C28" s="53" t="s">
+      <c r="C28" s="52" t="s">
         <v>224</v>
       </c>
-      <c r="D28" s="53"/>
-      <c r="E28" s="53"/>
-      <c r="F28" s="53"/>
-      <c r="G28" s="53"/>
+      <c r="D28" s="52"/>
+      <c r="E28" s="52"/>
+      <c r="F28" s="52"/>
+      <c r="G28" s="52"/>
     </row>
     <row r="29" spans="1:7" ht="15.75" customHeight="1">
-      <c r="A29" s="53" t="s">
+      <c r="A29" s="52" t="s">
         <v>177</v>
       </c>
-      <c r="B29" s="53" t="s">
+      <c r="B29" s="52" t="s">
         <v>197</v>
       </c>
-      <c r="C29" s="53" t="s">
+      <c r="C29" s="52" t="s">
         <v>197</v>
       </c>
-      <c r="D29" s="53"/>
-      <c r="E29" s="53"/>
-      <c r="F29" s="53"/>
-      <c r="G29" s="53"/>
+      <c r="D29" s="52"/>
+      <c r="E29" s="52"/>
+      <c r="F29" s="52"/>
+      <c r="G29" s="52"/>
     </row>
     <row r="30" spans="1:7" ht="15.75" customHeight="1">
-      <c r="A30" s="53" t="s">
+      <c r="A30" s="52" t="s">
         <v>196</v>
       </c>
-      <c r="B30" s="53" t="s">
+      <c r="B30" s="52" t="s">
         <v>189</v>
       </c>
-      <c r="C30" s="53" t="s">
+      <c r="C30" s="52" t="s">
         <v>193</v>
       </c>
-      <c r="D30" s="53"/>
-      <c r="E30" s="53"/>
-      <c r="F30" s="53"/>
-      <c r="G30" s="53"/>
+      <c r="D30" s="52"/>
+      <c r="E30" s="52"/>
+      <c r="F30" s="52"/>
+      <c r="G30" s="52"/>
     </row>
     <row r="31" spans="1:7" ht="15.75" customHeight="1">
-      <c r="A31" s="53" t="s">
+      <c r="A31" s="52" t="s">
         <v>208</v>
       </c>
-      <c r="B31" s="53" t="s">
+      <c r="B31" s="52" t="s">
         <v>196</v>
       </c>
-      <c r="D31" s="53"/>
-      <c r="E31" s="53"/>
-      <c r="F31" s="53"/>
-      <c r="G31" s="53"/>
+      <c r="D31" s="52"/>
+      <c r="E31" s="52"/>
+      <c r="F31" s="52"/>
+      <c r="G31" s="52"/>
     </row>
     <row r="32" spans="1:7" ht="15.75" customHeight="1">
-      <c r="A32" s="53" t="s">
+      <c r="A32" s="52" t="s">
         <v>193</v>
       </c>
-      <c r="B32" s="53" t="s">
+      <c r="B32" s="52" t="s">
         <v>208</v>
       </c>
-      <c r="C32" s="53"/>
-      <c r="D32" s="53"/>
-      <c r="E32" s="53"/>
-      <c r="F32" s="53"/>
-      <c r="G32" s="53"/>
+      <c r="C32" s="52"/>
+      <c r="D32" s="52"/>
+      <c r="E32" s="52"/>
+      <c r="F32" s="52"/>
+      <c r="G32" s="52"/>
     </row>
     <row r="33" spans="1:7" ht="15.75" customHeight="1">
-      <c r="A33" s="53"/>
-      <c r="B33" s="53" t="s">
+      <c r="A33" s="52"/>
+      <c r="B33" s="52" t="s">
         <v>193</v>
       </c>
-      <c r="D33" s="53"/>
-      <c r="E33" s="53"/>
-      <c r="F33" s="53"/>
-      <c r="G33" s="53"/>
+      <c r="D33" s="52"/>
+      <c r="E33" s="52"/>
+      <c r="F33" s="52"/>
+      <c r="G33" s="52"/>
     </row>
     <row r="34" spans="1:7" ht="15.75" customHeight="1">
-      <c r="A34" s="53"/>
-      <c r="B34" s="53"/>
-      <c r="C34" s="53"/>
-      <c r="D34" s="53"/>
-      <c r="E34" s="53"/>
-      <c r="F34" s="53"/>
-      <c r="G34" s="53"/>
+      <c r="A34" s="52"/>
+      <c r="B34" s="52"/>
+      <c r="C34" s="52"/>
+      <c r="D34" s="52"/>
+      <c r="E34" s="52"/>
+      <c r="F34" s="52"/>
+      <c r="G34" s="52"/>
     </row>
     <row r="35" spans="1:7" ht="15.75" customHeight="1">
-      <c r="A35" s="53"/>
-      <c r="B35" s="53"/>
-      <c r="C35" s="53"/>
-      <c r="D35" s="53"/>
-      <c r="E35" s="53"/>
-      <c r="F35" s="53"/>
-      <c r="G35" s="53"/>
+      <c r="A35" s="52"/>
+      <c r="B35" s="52"/>
+      <c r="C35" s="52"/>
+      <c r="D35" s="52"/>
+      <c r="E35" s="52"/>
+      <c r="F35" s="52"/>
+      <c r="G35" s="52"/>
     </row>
     <row r="36" spans="1:7" ht="15.75" customHeight="1">
-      <c r="A36" s="53"/>
-      <c r="B36" s="53"/>
-      <c r="C36" s="53"/>
-      <c r="D36" s="53"/>
-      <c r="E36" s="53"/>
-      <c r="F36" s="53"/>
-      <c r="G36" s="53"/>
+      <c r="A36" s="52"/>
+      <c r="B36" s="52"/>
+      <c r="C36" s="52"/>
+      <c r="D36" s="52"/>
+      <c r="E36" s="52"/>
+      <c r="F36" s="52"/>
+      <c r="G36" s="52"/>
     </row>
     <row r="37" spans="1:7" ht="15.75" customHeight="1"/>
     <row r="38" spans="1:7" ht="15.75" customHeight="1"/>

</xml_diff>

<commit_message>
Implementaciones definitivas en la funcion de Configuracion de Alarmas para el anexo y checklist
</commit_message>
<xml_diff>
--- a/devops-powershell/reportes/templete/Checklist Proactiva Actualizada - Cliente - Mes.xlsx
+++ b/devops-powershell/reportes/templete/Checklist Proactiva Actualizada - Cliente - Mes.xlsx
@@ -792,7 +792,7 @@
     </font>
     <font>
       <sz val="11"/>
-      <color theme="10"/>
+      <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
     </font>
@@ -952,7 +952,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="56">
+  <cellXfs count="57">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -1081,6 +1081,7 @@
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyProtection="1"/>
     <xf numFmtId="0" fontId="8" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="8" fillId="5" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1299,7 +1300,7 @@
   <dimension ref="A1:Z987"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="C3" workbookViewId="0">
-      <selection activeCell="G15" sqref="G15"/>
+      <selection activeCell="G27" sqref="G27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
@@ -1724,7 +1725,7 @@
         <v>36</v>
       </c>
       <c r="G11" s="19"/>
-      <c r="H11" s="19"/>
+      <c r="H11" s="55"/>
       <c r="I11" s="18"/>
       <c r="J11" s="20"/>
       <c r="K11" s="20"/>
@@ -1764,7 +1765,7 @@
         <v>36</v>
       </c>
       <c r="G12" s="19"/>
-      <c r="H12" s="19"/>
+      <c r="H12" s="55"/>
       <c r="I12" s="18"/>
       <c r="J12" s="20"/>
       <c r="K12" s="20"/>
@@ -1804,7 +1805,7 @@
         <v>36</v>
       </c>
       <c r="G13" s="19"/>
-      <c r="H13" s="19"/>
+      <c r="H13" s="55"/>
       <c r="I13" s="18"/>
       <c r="J13" s="20"/>
       <c r="K13" s="20"/>
@@ -1884,7 +1885,7 @@
         <v>36</v>
       </c>
       <c r="G15" s="19"/>
-      <c r="H15" s="19"/>
+      <c r="H15" s="55"/>
       <c r="I15" s="18"/>
       <c r="J15" s="20"/>
       <c r="K15" s="20"/>
@@ -1924,7 +1925,7 @@
         <v>36</v>
       </c>
       <c r="G16" s="19"/>
-      <c r="H16" s="19"/>
+      <c r="H16" s="55"/>
       <c r="I16" s="18"/>
       <c r="J16" s="20"/>
       <c r="K16" s="20"/>
@@ -1964,7 +1965,7 @@
         <v>36</v>
       </c>
       <c r="G17" s="19"/>
-      <c r="H17" s="19"/>
+      <c r="H17" s="55"/>
       <c r="I17" s="18"/>
       <c r="J17" s="20"/>
       <c r="K17" s="20"/>
@@ -2004,7 +2005,7 @@
         <v>36</v>
       </c>
       <c r="G18" s="19"/>
-      <c r="H18" s="19"/>
+      <c r="H18" s="55"/>
       <c r="I18" s="18"/>
       <c r="J18" s="20"/>
       <c r="K18" s="20"/>
@@ -2044,7 +2045,7 @@
         <v>36</v>
       </c>
       <c r="G19" s="25"/>
-      <c r="H19" s="25"/>
+      <c r="H19" s="56"/>
       <c r="I19" s="24"/>
       <c r="J19" s="20"/>
       <c r="K19" s="20"/>

</xml_diff>